<commit_message>
update tests and examples
</commit_message>
<xml_diff>
--- a/Examples/SelectingModuleandInverterExample/pySAM_Pvsamv1_default_values.xlsx
+++ b/Examples/SelectingModuleandInverterExample/pySAM_Pvsamv1_default_values.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="584">
   <si>
     <t>AdjustmentFactors</t>
   </si>
@@ -148,9 +148,15 @@
     <t>cec_module_length</t>
   </si>
   <si>
+    <t>1.559</t>
+  </si>
+  <si>
     <t>cec_module_width</t>
   </si>
   <si>
+    <t>1.046</t>
+  </si>
+  <si>
     <t>cec_mounting_config</t>
   </si>
   <si>
@@ -214,9 +220,6 @@
     <t>sixpar_aisc</t>
   </si>
   <si>
-    <t>0.004</t>
-  </si>
-  <si>
     <t>sixpar_area</t>
   </si>
   <si>
@@ -232,9 +235,6 @@
     <t>sixpar_bvoc</t>
   </si>
   <si>
-    <t>-0.11</t>
-  </si>
-  <si>
     <t>sixpar_celltech</t>
   </si>
   <si>
@@ -601,19 +601,19 @@
     <t>inv_snl_eff_cec</t>
   </si>
   <si>
-    <t>98.2262</t>
+    <t>98.6909</t>
   </si>
   <si>
     <t>inv_snl_paco</t>
   </si>
   <si>
-    <t>60033.0</t>
+    <t>226997.0</t>
   </si>
   <si>
     <t>inverter_count</t>
   </si>
   <si>
-    <t>7.0</t>
+    <t>2.0</t>
   </si>
   <si>
     <t>inverter_model</t>
@@ -691,7 +691,7 @@
     <t>inv_tdc_cec_cg</t>
   </si>
   <si>
-    <t>((1300.0, 50.0, -0.02, 53.0, -0.47),)</t>
+    <t>((1500.0, 50.0, -0.02, 53.0, -0.47),)</t>
   </si>
   <si>
     <t>InverterCECDatabase</t>
@@ -700,52 +700,55 @@
     <t>inv_snl_c0</t>
   </si>
   <si>
-    <t>-1.41816e-07</t>
+    <t>-4.38534e-08</t>
   </si>
   <si>
     <t>inv_snl_c1</t>
   </si>
   <si>
-    <t>-3.03226e-05</t>
+    <t>-8.57136e-06</t>
   </si>
   <si>
     <t>inv_snl_c2</t>
   </si>
   <si>
-    <t>0.0010953</t>
+    <t>-0.000791432</t>
   </si>
   <si>
     <t>inv_snl_c3</t>
   </si>
   <si>
-    <t>-0.000176618</t>
+    <t>-0.000320828</t>
   </si>
   <si>
     <t>inv_snl_pdco</t>
   </si>
   <si>
-    <t>61147.2</t>
+    <t>230396.0</t>
   </si>
   <si>
     <t>inv_snl_pnt</t>
   </si>
   <si>
-    <t>0.9</t>
+    <t>5.21</t>
   </si>
   <si>
     <t>inv_snl_pso</t>
   </si>
   <si>
-    <t>148.792</t>
+    <t>443.342</t>
   </si>
   <si>
     <t>inv_snl_vdcmax</t>
   </si>
   <si>
+    <t>1300.0</t>
+  </si>
+  <si>
     <t>inv_snl_vdco</t>
   </si>
   <si>
-    <t>720.0</t>
+    <t>1080.0</t>
   </si>
   <si>
     <t>inv_tdc_cec_db</t>
@@ -814,7 +817,7 @@
     <t>module_aspect_ratio</t>
   </si>
   <si>
-    <t>1.7</t>
+    <t>1.49044</t>
   </si>
   <si>
     <t>subarray1_mod_orient</t>
@@ -829,9 +832,6 @@
     <t>subarray1_nmody</t>
   </si>
   <si>
-    <t>2.0</t>
-  </si>
-  <si>
     <t>subarray2_mod_orient</t>
   </si>
   <si>
@@ -952,6 +952,9 @@
     <t>subarray1_rack_shading</t>
   </si>
   <si>
+    <t>4.0</t>
+  </si>
+  <si>
     <t>subarray1_rear_soiling_loss</t>
   </si>
   <si>
@@ -1066,6 +1069,12 @@
     <t>Outputs</t>
   </si>
   <si>
+    <t>PVLosses</t>
+  </si>
+  <si>
+    <t>enable_subhourly_clipping</t>
+  </si>
+  <si>
     <t>PriceSignal</t>
   </si>
   <si>
@@ -1084,31 +1093,31 @@
     <t>snl_a0</t>
   </si>
   <si>
-    <t>0.94045</t>
+    <t>0.9597</t>
   </si>
   <si>
     <t>snl_a1</t>
   </si>
   <si>
-    <t>0.052641</t>
+    <t>0.03217</t>
   </si>
   <si>
     <t>snl_a2</t>
   </si>
   <si>
-    <t>-0.0093897</t>
+    <t>-0.00366</t>
   </si>
   <si>
     <t>snl_a3</t>
   </si>
   <si>
-    <t>0.00072623</t>
+    <t>6e-05</t>
   </si>
   <si>
     <t>snl_a4</t>
   </si>
   <si>
-    <t>-1.9938e-05</t>
+    <t>5.4e-06</t>
   </si>
   <si>
     <t>snl_aimp</t>
@@ -1120,15 +1129,12 @@
     <t>snl_aisc</t>
   </si>
   <si>
-    <t>0.00061</t>
+    <t>0.00059</t>
   </si>
   <si>
     <t>snl_area</t>
   </si>
   <si>
-    <t>1.244</t>
-  </si>
-  <si>
     <t>snl_b</t>
   </si>
   <si>
@@ -1147,7 +1153,7 @@
     <t>snl_b2</t>
   </si>
   <si>
-    <t>0.0003103</t>
+    <t>0.00031</t>
   </si>
   <si>
     <t>snl_b3</t>
@@ -1171,61 +1177,61 @@
     <t>snl_bvmpo</t>
   </si>
   <si>
-    <t>-0.139</t>
+    <t>-0.186</t>
   </si>
   <si>
     <t>snl_bvoco</t>
   </si>
   <si>
-    <t>-0.136</t>
+    <t>-0.177</t>
   </si>
   <si>
     <t>snl_c0</t>
   </si>
   <si>
-    <t>1.0039</t>
+    <t>1.009</t>
   </si>
   <si>
     <t>snl_c1</t>
   </si>
   <si>
-    <t>-0.0039</t>
+    <t>-0.009</t>
   </si>
   <si>
     <t>snl_c2</t>
   </si>
   <si>
-    <t>0.291066</t>
+    <t>0.3802</t>
   </si>
   <si>
     <t>snl_c3</t>
   </si>
   <si>
-    <t>-4.73546</t>
+    <t>-3.716</t>
   </si>
   <si>
     <t>snl_c4</t>
   </si>
   <si>
-    <t>0.9942</t>
+    <t>0.988</t>
   </si>
   <si>
     <t>snl_c5</t>
   </si>
   <si>
-    <t>0.0058</t>
+    <t>0.012</t>
   </si>
   <si>
     <t>snl_c6</t>
   </si>
   <si>
-    <t>1.0723</t>
+    <t>1.093</t>
   </si>
   <si>
     <t>snl_c7</t>
   </si>
   <si>
-    <t>-0.0723</t>
+    <t>-0.093</t>
   </si>
   <si>
     <t>snl_dtc</t>
@@ -1240,25 +1246,25 @@
     <t>snl_impo</t>
   </si>
   <si>
-    <t>5.25</t>
+    <t>5.58</t>
   </si>
   <si>
     <t>snl_isco</t>
   </si>
   <si>
-    <t>5.75</t>
+    <t>5.96</t>
   </si>
   <si>
     <t>snl_ixo</t>
   </si>
   <si>
-    <t>5.65</t>
+    <t>5.9</t>
   </si>
   <si>
     <t>snl_ixxo</t>
   </si>
   <si>
-    <t>3.85</t>
+    <t>4.1</t>
   </si>
   <si>
     <t>snl_mbvmp</t>
@@ -1273,7 +1279,7 @@
     <t>snl_n</t>
   </si>
   <si>
-    <t>1.221</t>
+    <t>1.131</t>
   </si>
   <si>
     <t>snl_ref_a</t>
@@ -1288,22 +1294,16 @@
     <t>snl_series_cells</t>
   </si>
   <si>
-    <t>72.0</t>
-  </si>
-  <si>
     <t>snl_transient_thermal_model_unit_mass</t>
   </si>
   <si>
     <t>snl_vmpo</t>
   </si>
   <si>
-    <t>40.0</t>
-  </si>
-  <si>
     <t>snl_voco</t>
   </si>
   <si>
-    <t>47.7</t>
+    <t>64.2</t>
   </si>
   <si>
     <t>Shading</t>
@@ -1312,15 +1312,138 @@
     <t>subarray1_shade_mode</t>
   </si>
   <si>
+    <t>subarray1_shading_azal</t>
+  </si>
+  <si>
+    <t>((0.0,),)</t>
+  </si>
+  <si>
+    <t>subarray1_shading_diff</t>
+  </si>
+  <si>
+    <t>subarray1_shading_en_azal</t>
+  </si>
+  <si>
+    <t>subarray1_shading_en_diff</t>
+  </si>
+  <si>
+    <t>subarray1_shading_en_mxh</t>
+  </si>
+  <si>
+    <t>subarray1_shading_en_string_option</t>
+  </si>
+  <si>
+    <t>subarray1_shading_en_timestep</t>
+  </si>
+  <si>
+    <t>subarray1_shading_mxh</t>
+  </si>
+  <si>
+    <t>subarray1_shading_string_option</t>
+  </si>
+  <si>
+    <t>subarray1_shading_timestep</t>
+  </si>
+  <si>
     <t>subarray2_shade_mode</t>
   </si>
   <si>
+    <t>subarray2_shading_azal</t>
+  </si>
+  <si>
+    <t>subarray2_shading_diff</t>
+  </si>
+  <si>
+    <t>subarray2_shading_en_azal</t>
+  </si>
+  <si>
+    <t>subarray2_shading_en_diff</t>
+  </si>
+  <si>
+    <t>subarray2_shading_en_mxh</t>
+  </si>
+  <si>
+    <t>subarray2_shading_en_string_option</t>
+  </si>
+  <si>
+    <t>subarray2_shading_en_timestep</t>
+  </si>
+  <si>
+    <t>subarray2_shading_mxh</t>
+  </si>
+  <si>
+    <t>subarray2_shading_string_option</t>
+  </si>
+  <si>
+    <t>subarray2_shading_timestep</t>
+  </si>
+  <si>
     <t>subarray3_shade_mode</t>
   </si>
   <si>
+    <t>subarray3_shading_azal</t>
+  </si>
+  <si>
+    <t>subarray3_shading_diff</t>
+  </si>
+  <si>
+    <t>subarray3_shading_en_azal</t>
+  </si>
+  <si>
+    <t>subarray3_shading_en_diff</t>
+  </si>
+  <si>
+    <t>subarray3_shading_en_mxh</t>
+  </si>
+  <si>
+    <t>subarray3_shading_en_string_option</t>
+  </si>
+  <si>
+    <t>subarray3_shading_en_timestep</t>
+  </si>
+  <si>
+    <t>subarray3_shading_mxh</t>
+  </si>
+  <si>
+    <t>subarray3_shading_string_option</t>
+  </si>
+  <si>
+    <t>subarray3_shading_timestep</t>
+  </si>
+  <si>
     <t>subarray4_shade_mode</t>
   </si>
   <si>
+    <t>subarray4_shading_azal</t>
+  </si>
+  <si>
+    <t>subarray4_shading_diff</t>
+  </si>
+  <si>
+    <t>subarray4_shading_en_azal</t>
+  </si>
+  <si>
+    <t>subarray4_shading_en_diff</t>
+  </si>
+  <si>
+    <t>subarray4_shading_en_mxh</t>
+  </si>
+  <si>
+    <t>subarray4_shading_en_string_option</t>
+  </si>
+  <si>
+    <t>subarray4_shading_en_timestep</t>
+  </si>
+  <si>
+    <t>subarray4_shading_mxh</t>
+  </si>
+  <si>
+    <t>subarray4_shading_string_option</t>
+  </si>
+  <si>
+    <t>subarray4_shading_timestep</t>
+  </si>
+  <si>
     <t>SimpleEfficiencyModuleModel</t>
   </si>
   <si>
@@ -1405,9 +1528,6 @@
     <t>spe_reference</t>
   </si>
   <si>
-    <t>4.0</t>
-  </si>
-  <si>
     <t>spe_temp_coeff</t>
   </si>
   <si>
@@ -1480,9 +1600,6 @@
     <t>subarray1_modules_per_string</t>
   </si>
   <si>
-    <t>13.0</t>
-  </si>
-  <si>
     <t>subarray1_monthly_tilt</t>
   </si>
   <si>
@@ -1495,7 +1612,7 @@
     <t>subarray1_nstrings</t>
   </si>
   <si>
-    <t>124.0</t>
+    <t>81.0</t>
   </si>
   <si>
     <t>subarray1_rotlim</t>
@@ -1648,7 +1765,7 @@
     <t>system_capacity</t>
   </si>
   <si>
-    <t>499.96</t>
+    <t>502.441</t>
   </si>
 </sst>
 </file>
@@ -1980,7 +2097,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C393"/>
+  <dimension ref="A2:C435"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2180,20 +2297,20 @@
         <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="2:3">
       <c r="B28" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="2:3">
       <c r="B29" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
@@ -2201,7 +2318,7 @@
     </row>
     <row r="30" spans="2:3">
       <c r="B30" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
         <v>5</v>
@@ -2209,47 +2326,47 @@
     </row>
     <row r="31" spans="2:3">
       <c r="B31" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C31" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="2:3">
       <c r="B32" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="B33" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="B34" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C34" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="B35" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="B36" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
@@ -2257,42 +2374,42 @@
     </row>
     <row r="37" spans="1:3">
       <c r="B37" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C37" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="B38" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C38" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="B39" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C39" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C41" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="B42" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C42" t="s">
         <v>14</v>
@@ -2300,7 +2417,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="B43" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C43" t="s">
         <v>18</v>
@@ -2308,7 +2425,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="B44" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C44" t="s">
         <v>25</v>
@@ -2316,7 +2433,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="B45" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C45" t="s">
         <v>27</v>
@@ -2324,10 +2441,10 @@
     </row>
     <row r="46" spans="1:3">
       <c r="B46" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C46" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -2383,7 +2500,7 @@
         <v>79</v>
       </c>
       <c r="C53" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -2391,7 +2508,7 @@
         <v>80</v>
       </c>
       <c r="C54" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -2399,7 +2516,7 @@
         <v>81</v>
       </c>
       <c r="C55" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -2407,7 +2524,7 @@
         <v>82</v>
       </c>
       <c r="C56" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -2415,7 +2532,7 @@
         <v>83</v>
       </c>
       <c r="C57" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -2423,7 +2540,7 @@
         <v>84</v>
       </c>
       <c r="C58" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -2861,7 +2978,7 @@
         <v>178</v>
       </c>
       <c r="C115" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2869,7 +2986,7 @@
         <v>179</v>
       </c>
       <c r="C116" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2904,7 +3021,7 @@
         <v>187</v>
       </c>
       <c r="C121" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -3150,20 +3267,20 @@
         <v>241</v>
       </c>
       <c r="C153" t="s">
-        <v>202</v>
+        <v>242</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="B154" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C154" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="B155" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C155" t="s">
         <v>225</v>
@@ -3171,13 +3288,13 @@
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B157" t="s">
         <v>187</v>
       </c>
       <c r="C157" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -3190,7 +3307,7 @@
     </row>
     <row r="159" spans="1:3">
       <c r="B159" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C159" t="s">
         <v>18</v>
@@ -3198,7 +3315,7 @@
     </row>
     <row r="160" spans="1:3">
       <c r="B160" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C160" t="s">
         <v>5</v>
@@ -3206,7 +3323,7 @@
     </row>
     <row r="161" spans="1:3">
       <c r="B161" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C161" t="s">
         <v>221</v>
@@ -3214,15 +3331,15 @@
     </row>
     <row r="162" spans="1:3">
       <c r="B162" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C162" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="B163" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C163" t="s">
         <v>225</v>
@@ -3230,18 +3347,18 @@
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B166" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C166" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -3254,23 +3371,23 @@
     </row>
     <row r="168" spans="1:3">
       <c r="B168" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C168" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="B169" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C169" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="B170" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C170" t="s">
         <v>5</v>
@@ -3278,7 +3395,7 @@
     </row>
     <row r="171" spans="1:3">
       <c r="B171" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C171" t="s">
         <v>221</v>
@@ -3286,15 +3403,15 @@
     </row>
     <row r="172" spans="1:3">
       <c r="B172" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C172" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="B173" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C173" t="s">
         <v>225</v>
@@ -3302,18 +3419,18 @@
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B175" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C175" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="B176" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C176" t="s">
         <v>5</v>
@@ -3321,18 +3438,18 @@
     </row>
     <row r="177" spans="1:3">
       <c r="B177" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C177" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="B178" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C178" t="s">
-        <v>271</v>
+        <v>199</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -3356,7 +3473,7 @@
         <v>275</v>
       </c>
       <c r="C181" t="s">
-        <v>271</v>
+        <v>199</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -3380,7 +3497,7 @@
         <v>278</v>
       </c>
       <c r="C184" t="s">
-        <v>271</v>
+        <v>199</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -3404,7 +3521,7 @@
         <v>281</v>
       </c>
       <c r="C187" t="s">
-        <v>271</v>
+        <v>199</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -3549,7 +3666,7 @@
         <v>305</v>
       </c>
       <c r="C207" t="s">
-        <v>271</v>
+        <v>199</v>
       </c>
     </row>
     <row r="208" spans="1:3">
@@ -3573,7 +3690,7 @@
         <v>309</v>
       </c>
       <c r="C210" t="s">
-        <v>271</v>
+        <v>199</v>
       </c>
     </row>
     <row r="211" spans="2:3">
@@ -3589,12 +3706,12 @@
         <v>311</v>
       </c>
       <c r="C212" t="s">
-        <v>5</v>
+        <v>312</v>
       </c>
     </row>
     <row r="213" spans="2:3">
       <c r="B213" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C213" t="s">
         <v>5</v>
@@ -3602,15 +3719,15 @@
     </row>
     <row r="214" spans="2:3">
       <c r="B214" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C214" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="215" spans="2:3">
       <c r="B215" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C215" t="s">
         <v>5</v>
@@ -3618,15 +3735,15 @@
     </row>
     <row r="216" spans="2:3">
       <c r="B216" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C216" t="s">
-        <v>271</v>
+        <v>199</v>
       </c>
     </row>
     <row r="217" spans="2:3">
       <c r="B217" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C217" t="s">
         <v>307</v>
@@ -3634,7 +3751,7 @@
     </row>
     <row r="218" spans="2:3">
       <c r="B218" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C218" t="s">
         <v>5</v>
@@ -3642,15 +3759,15 @@
     </row>
     <row r="219" spans="2:3">
       <c r="B219" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C219" t="s">
-        <v>271</v>
+        <v>199</v>
       </c>
     </row>
     <row r="220" spans="2:3">
       <c r="B220" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C220" t="s">
         <v>5</v>
@@ -3658,7 +3775,7 @@
     </row>
     <row r="221" spans="2:3">
       <c r="B221" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C221" t="s">
         <v>5</v>
@@ -3666,7 +3783,7 @@
     </row>
     <row r="222" spans="2:3">
       <c r="B222" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C222" t="s">
         <v>5</v>
@@ -3674,15 +3791,15 @@
     </row>
     <row r="223" spans="2:3">
       <c r="B223" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C223" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="224" spans="2:3">
       <c r="B224" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C224" t="s">
         <v>5</v>
@@ -3690,15 +3807,15 @@
     </row>
     <row r="225" spans="2:3">
       <c r="B225" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C225" t="s">
-        <v>271</v>
+        <v>199</v>
       </c>
     </row>
     <row r="226" spans="2:3">
       <c r="B226" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C226" t="s">
         <v>307</v>
@@ -3706,7 +3823,7 @@
     </row>
     <row r="227" spans="2:3">
       <c r="B227" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C227" t="s">
         <v>5</v>
@@ -3714,15 +3831,15 @@
     </row>
     <row r="228" spans="2:3">
       <c r="B228" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C228" t="s">
-        <v>271</v>
+        <v>199</v>
       </c>
     </row>
     <row r="229" spans="2:3">
       <c r="B229" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C229" t="s">
         <v>5</v>
@@ -3730,7 +3847,7 @@
     </row>
     <row r="230" spans="2:3">
       <c r="B230" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C230" t="s">
         <v>5</v>
@@ -3738,7 +3855,7 @@
     </row>
     <row r="231" spans="2:3">
       <c r="B231" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C231" t="s">
         <v>5</v>
@@ -3746,15 +3863,15 @@
     </row>
     <row r="232" spans="2:3">
       <c r="B232" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C232" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="233" spans="2:3">
       <c r="B233" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C233" t="s">
         <v>5</v>
@@ -3762,15 +3879,15 @@
     </row>
     <row r="234" spans="2:3">
       <c r="B234" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C234" t="s">
-        <v>271</v>
+        <v>199</v>
       </c>
     </row>
     <row r="235" spans="2:3">
       <c r="B235" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C235" t="s">
         <v>307</v>
@@ -3778,7 +3895,7 @@
     </row>
     <row r="236" spans="2:3">
       <c r="B236" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C236" t="s">
         <v>5</v>
@@ -3786,15 +3903,15 @@
     </row>
     <row r="237" spans="2:3">
       <c r="B237" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C237" t="s">
-        <v>271</v>
+        <v>199</v>
       </c>
     </row>
     <row r="238" spans="2:3">
       <c r="B238" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C238" t="s">
         <v>5</v>
@@ -3802,7 +3919,7 @@
     </row>
     <row r="239" spans="2:3">
       <c r="B239" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C239" t="s">
         <v>5</v>
@@ -3810,7 +3927,7 @@
     </row>
     <row r="240" spans="2:3">
       <c r="B240" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C240" t="s">
         <v>5</v>
@@ -3818,15 +3935,15 @@
     </row>
     <row r="241" spans="1:3">
       <c r="B241" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C241" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="B242" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C242" t="s">
         <v>5</v>
@@ -3834,7 +3951,7 @@
     </row>
     <row r="243" spans="1:3">
       <c r="B243" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C243" t="s">
         <v>5</v>
@@ -3842,7 +3959,7 @@
     </row>
     <row r="244" spans="1:3">
       <c r="B244" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C244" t="s">
         <v>5</v>
@@ -3850,7 +3967,7 @@
     </row>
     <row r="245" spans="1:3">
       <c r="B245" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C245" t="s">
         <v>5</v>
@@ -3858,15 +3975,15 @@
     </row>
     <row r="247" spans="1:3">
       <c r="A247" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B248" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C248" t="s">
         <v>18</v>
@@ -3874,292 +3991,287 @@
     </row>
     <row r="250" spans="1:3">
       <c r="A250" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="251" spans="1:3">
       <c r="A251" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3">
-      <c r="A252" t="s">
         <v>351</v>
+      </c>
+      <c r="B251" t="s">
+        <v>352</v>
+      </c>
+      <c r="C251" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="253" spans="1:3">
       <c r="A253" t="s">
-        <v>352</v>
-      </c>
-      <c r="B253" t="s">
         <v>353</v>
       </c>
-      <c r="C253" t="s">
+    </row>
+    <row r="254" spans="1:3">
+      <c r="A254" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="254" spans="1:3">
-      <c r="B254" t="s">
+    <row r="255" spans="1:3">
+      <c r="A255" t="s">
         <v>355</v>
       </c>
-      <c r="C254" t="s">
+      <c r="B255" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="255" spans="1:3">
-      <c r="B255" t="s">
+      <c r="C255" t="s">
         <v>357</v>
-      </c>
-      <c r="C255" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="B256" t="s">
+        <v>358</v>
+      </c>
+      <c r="C256" t="s">
         <v>359</v>
-      </c>
-      <c r="C256" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="257" spans="2:3">
       <c r="B257" t="s">
+        <v>360</v>
+      </c>
+      <c r="C257" t="s">
         <v>361</v>
-      </c>
-      <c r="C257" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="258" spans="2:3">
       <c r="B258" t="s">
+        <v>362</v>
+      </c>
+      <c r="C258" t="s">
         <v>363</v>
-      </c>
-      <c r="C258" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="259" spans="2:3">
       <c r="B259" t="s">
+        <v>364</v>
+      </c>
+      <c r="C259" t="s">
         <v>365</v>
-      </c>
-      <c r="C259" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="260" spans="2:3">
       <c r="B260" t="s">
+        <v>366</v>
+      </c>
+      <c r="C260" t="s">
         <v>367</v>
-      </c>
-      <c r="C260" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="261" spans="2:3">
       <c r="B261" t="s">
+        <v>368</v>
+      </c>
+      <c r="C261" t="s">
         <v>369</v>
-      </c>
-      <c r="C261" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="262" spans="2:3">
       <c r="B262" t="s">
+        <v>370</v>
+      </c>
+      <c r="C262" t="s">
         <v>371</v>
-      </c>
-      <c r="C262" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="263" spans="2:3">
       <c r="B263" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C263" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="264" spans="2:3">
       <c r="B264" t="s">
+        <v>373</v>
+      </c>
+      <c r="C264" t="s">
         <v>374</v>
-      </c>
-      <c r="C264" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="265" spans="2:3">
       <c r="B265" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C265" t="s">
-        <v>377</v>
+        <v>18</v>
       </c>
     </row>
     <row r="266" spans="2:3">
       <c r="B266" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C266" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="267" spans="2:3">
       <c r="B267" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C267" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="268" spans="2:3">
       <c r="B268" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C268" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="269" spans="2:3">
       <c r="B269" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C269" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="270" spans="2:3">
       <c r="B270" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C270" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="271" spans="2:3">
       <c r="B271" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C271" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="272" spans="2:3">
       <c r="B272" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C272" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="273" spans="2:3">
       <c r="B273" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C273" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="274" spans="2:3">
       <c r="B274" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C274" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="275" spans="2:3">
       <c r="B275" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C275" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="276" spans="2:3">
       <c r="B276" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C276" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="277" spans="2:3">
       <c r="B277" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C277" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="278" spans="2:3">
       <c r="B278" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C278" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="279" spans="2:3">
       <c r="B279" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C279" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="280" spans="2:3">
       <c r="B280" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C280" t="s">
-        <v>18</v>
+        <v>405</v>
       </c>
     </row>
     <row r="281" spans="2:3">
       <c r="B281" t="s">
+        <v>406</v>
+      </c>
+      <c r="C281" t="s">
         <v>407</v>
-      </c>
-      <c r="C281" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="282" spans="2:3">
       <c r="B282" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C282" t="s">
-        <v>410</v>
+        <v>18</v>
       </c>
     </row>
     <row r="283" spans="2:3">
       <c r="B283" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C283" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="284" spans="2:3">
       <c r="B284" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C284" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="285" spans="2:3">
       <c r="B285" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C285" t="s">
-        <v>5</v>
+        <v>414</v>
       </c>
     </row>
     <row r="286" spans="2:3">
       <c r="B286" t="s">
+        <v>415</v>
+      </c>
+      <c r="C286" t="s">
         <v>416</v>
-      </c>
-      <c r="C286" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="287" spans="2:3">
@@ -4175,23 +4287,23 @@
         <v>418</v>
       </c>
       <c r="C288" t="s">
-        <v>419</v>
+        <v>5</v>
       </c>
     </row>
     <row r="289" spans="1:3">
       <c r="B289" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C289" t="s">
-        <v>354</v>
+        <v>5</v>
       </c>
     </row>
     <row r="290" spans="1:3">
       <c r="B290" t="s">
+        <v>420</v>
+      </c>
+      <c r="C290" t="s">
         <v>421</v>
-      </c>
-      <c r="C290" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="291" spans="1:3">
@@ -4199,7 +4311,7 @@
         <v>422</v>
       </c>
       <c r="C291" t="s">
-        <v>405</v>
+        <v>357</v>
       </c>
     </row>
     <row r="292" spans="1:3">
@@ -4207,55 +4319,55 @@
         <v>423</v>
       </c>
       <c r="C292" t="s">
-        <v>424</v>
+        <v>374</v>
       </c>
     </row>
     <row r="293" spans="1:3">
       <c r="B293" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C293" t="s">
-        <v>59</v>
+        <v>407</v>
       </c>
     </row>
     <row r="294" spans="1:3">
       <c r="B294" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C294" t="s">
-        <v>427</v>
+        <v>50</v>
       </c>
     </row>
     <row r="295" spans="1:3">
       <c r="B295" t="s">
+        <v>426</v>
+      </c>
+      <c r="C295" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3">
+      <c r="B296" t="s">
+        <v>427</v>
+      </c>
+      <c r="C296" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3">
+      <c r="B297" t="s">
         <v>428</v>
       </c>
-      <c r="C295" t="s">
+      <c r="C297" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="297" spans="1:3">
-      <c r="A297" t="s">
+    <row r="299" spans="1:3">
+      <c r="A299" t="s">
         <v>430</v>
       </c>
-      <c r="B297" t="s">
+      <c r="B299" t="s">
         <v>431</v>
-      </c>
-      <c r="C297" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="298" spans="1:3">
-      <c r="B298" t="s">
-        <v>432</v>
-      </c>
-      <c r="C298" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="299" spans="1:3">
-      <c r="B299" t="s">
-        <v>433</v>
       </c>
       <c r="C299" t="s">
         <v>5</v>
@@ -4263,122 +4375,127 @@
     </row>
     <row r="300" spans="1:3">
       <c r="B300" t="s">
+        <v>432</v>
+      </c>
+      <c r="C300" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3">
+      <c r="B301" t="s">
         <v>434</v>
       </c>
-      <c r="C300" t="s">
+      <c r="C301" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="302" spans="1:3">
-      <c r="A302" t="s">
+      <c r="B302" t="s">
         <v>435</v>
       </c>
-      <c r="B302" t="s">
-        <v>436</v>
-      </c>
       <c r="C302" t="s">
-        <v>437</v>
+        <v>5</v>
       </c>
     </row>
     <row r="303" spans="1:3">
       <c r="B303" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C303" t="s">
-        <v>439</v>
+        <v>5</v>
       </c>
     </row>
     <row r="304" spans="1:3">
       <c r="B304" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C304" t="s">
-        <v>372</v>
+        <v>5</v>
       </c>
     </row>
     <row r="305" spans="2:3">
       <c r="B305" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C305" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="306" spans="2:3">
       <c r="B306" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C306" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="307" spans="2:3">
       <c r="B307" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C307" t="s">
-        <v>27</v>
+        <v>433</v>
       </c>
     </row>
     <row r="308" spans="2:3">
       <c r="B308" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C308" t="s">
-        <v>405</v>
+        <v>5</v>
       </c>
     </row>
     <row r="309" spans="2:3">
       <c r="B309" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C309" t="s">
-        <v>446</v>
+        <v>433</v>
       </c>
     </row>
     <row r="310" spans="2:3">
       <c r="B310" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C310" t="s">
-        <v>446</v>
+        <v>5</v>
       </c>
     </row>
     <row r="311" spans="2:3">
       <c r="B311" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C311" t="s">
-        <v>446</v>
+        <v>433</v>
       </c>
     </row>
     <row r="312" spans="2:3">
       <c r="B312" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C312" t="s">
-        <v>446</v>
+        <v>5</v>
       </c>
     </row>
     <row r="313" spans="2:3">
       <c r="B313" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="C313" t="s">
-        <v>446</v>
+        <v>5</v>
       </c>
     </row>
     <row r="314" spans="2:3">
       <c r="B314" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C314" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="315" spans="2:3">
       <c r="B315" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="C315" t="s">
         <v>5</v>
@@ -4386,7 +4503,7 @@
     </row>
     <row r="316" spans="2:3">
       <c r="B316" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="C316" t="s">
         <v>5</v>
@@ -4394,320 +4511,330 @@
     </row>
     <row r="317" spans="2:3">
       <c r="B317" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C317" t="s">
-        <v>455</v>
+        <v>5</v>
       </c>
     </row>
     <row r="318" spans="2:3">
       <c r="B318" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C318" t="s">
-        <v>457</v>
+        <v>433</v>
       </c>
     </row>
     <row r="319" spans="2:3">
       <c r="B319" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="C319" t="s">
-        <v>221</v>
+        <v>5</v>
       </c>
     </row>
     <row r="320" spans="2:3">
       <c r="B320" t="s">
+        <v>453</v>
+      </c>
+      <c r="C320" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="321" spans="2:3">
+      <c r="B321" t="s">
+        <v>454</v>
+      </c>
+      <c r="C321" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="322" spans="2:3">
+      <c r="B322" t="s">
+        <v>455</v>
+      </c>
+      <c r="C322" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="323" spans="2:3">
+      <c r="B323" t="s">
+        <v>456</v>
+      </c>
+      <c r="C323" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="324" spans="2:3">
+      <c r="B324" t="s">
+        <v>457</v>
+      </c>
+      <c r="C324" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="325" spans="2:3">
+      <c r="B325" t="s">
+        <v>458</v>
+      </c>
+      <c r="C325" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="326" spans="2:3">
+      <c r="B326" t="s">
         <v>459</v>
       </c>
-      <c r="C320" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="321" spans="1:3">
-      <c r="B321" t="s">
+      <c r="C326" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="327" spans="2:3">
+      <c r="B327" t="s">
         <v>460</v>
       </c>
-      <c r="C321" t="s">
+      <c r="C327" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="328" spans="2:3">
+      <c r="B328" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="322" spans="1:3">
-      <c r="B322" t="s">
+      <c r="C328" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="329" spans="2:3">
+      <c r="B329" t="s">
         <v>462</v>
       </c>
-      <c r="C322" t="s">
+      <c r="C329" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="330" spans="2:3">
+      <c r="B330" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="323" spans="1:3">
-      <c r="B323" t="s">
+      <c r="C330" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="331" spans="2:3">
+      <c r="B331" t="s">
         <v>464</v>
       </c>
-      <c r="C323" t="s">
+      <c r="C331" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="332" spans="2:3">
+      <c r="B332" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="324" spans="1:3">
-      <c r="B324" t="s">
+      <c r="C332" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="333" spans="2:3">
+      <c r="B333" t="s">
         <v>466</v>
       </c>
-      <c r="C324" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="325" spans="1:3">
-      <c r="B325" t="s">
+      <c r="C333" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="334" spans="2:3">
+      <c r="B334" t="s">
         <v>467</v>
       </c>
-      <c r="C325" t="s">
+      <c r="C334" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="335" spans="2:3">
+      <c r="B335" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="327" spans="1:3">
-      <c r="A327" t="s">
+      <c r="C335" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="336" spans="2:3">
+      <c r="B336" t="s">
         <v>469</v>
       </c>
-      <c r="B327" t="s">
+      <c r="C336" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3">
+      <c r="B337" t="s">
         <v>470</v>
       </c>
-      <c r="C327" t="s">
+      <c r="C337" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3">
+      <c r="B338" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="328" spans="1:3">
-      <c r="B328" t="s">
+      <c r="C338" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3">
+      <c r="B339" t="s">
         <v>472</v>
       </c>
-      <c r="C328" t="s">
+      <c r="C339" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3">
+      <c r="B340" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="329" spans="1:3">
-      <c r="B329" t="s">
+      <c r="C340" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3">
+      <c r="B341" t="s">
         <v>474</v>
       </c>
-      <c r="C329" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="330" spans="1:3">
-      <c r="B330" t="s">
+      <c r="C341" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3">
+      <c r="B342" t="s">
         <v>475</v>
       </c>
-      <c r="C330" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="331" spans="1:3">
-      <c r="B331" t="s">
+      <c r="C342" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3">
+      <c r="A344" t="s">
         <v>476</v>
       </c>
-      <c r="C331" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="332" spans="1:3">
-      <c r="B332" t="s">
+      <c r="B344" t="s">
         <v>477</v>
       </c>
-      <c r="C332" t="s">
+      <c r="C344" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3">
+      <c r="B345" t="s">
+        <v>479</v>
+      </c>
+      <c r="C345" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3">
+      <c r="B346" t="s">
+        <v>481</v>
+      </c>
+      <c r="C346" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3">
+      <c r="B347" t="s">
+        <v>482</v>
+      </c>
+      <c r="C347" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="334" spans="1:3">
-      <c r="A334" t="s">
-        <v>478</v>
-      </c>
-      <c r="B334" t="s">
-        <v>479</v>
-      </c>
-      <c r="C334" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="336" spans="1:3">
-      <c r="A336" t="s">
-        <v>480</v>
-      </c>
-      <c r="B336" t="s">
-        <v>481</v>
-      </c>
-      <c r="C336" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="337" spans="2:3">
-      <c r="B337" t="s">
-        <v>198</v>
-      </c>
-      <c r="C337" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="338" spans="2:3">
-      <c r="B338" t="s">
-        <v>482</v>
-      </c>
-      <c r="C338" t="s">
+    <row r="348" spans="1:3">
+      <c r="B348" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="339" spans="2:3">
-      <c r="B339" t="s">
+      <c r="C348" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3">
+      <c r="B349" t="s">
         <v>484</v>
       </c>
-      <c r="C339" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="340" spans="2:3">
-      <c r="B340" t="s">
+      <c r="C349" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3">
+      <c r="B350" t="s">
         <v>485</v>
       </c>
-      <c r="C340" t="s">
+      <c r="C350" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3">
+      <c r="B351" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="341" spans="2:3">
-      <c r="B341" t="s">
+      <c r="C351" t="s">
         <v>487</v>
       </c>
-      <c r="C341" t="s">
+    </row>
+    <row r="352" spans="1:3">
+      <c r="B352" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="342" spans="2:3">
-      <c r="B342" t="s">
-        <v>489</v>
-      </c>
-      <c r="C342" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="343" spans="2:3">
-      <c r="B343" t="s">
-        <v>491</v>
-      </c>
-      <c r="C343" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="344" spans="2:3">
-      <c r="B344" t="s">
-        <v>492</v>
-      </c>
-      <c r="C344" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="345" spans="2:3">
-      <c r="B345" t="s">
-        <v>494</v>
-      </c>
-      <c r="C345" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="346" spans="2:3">
-      <c r="B346" t="s">
-        <v>496</v>
-      </c>
-      <c r="C346" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="347" spans="2:3">
-      <c r="B347" t="s">
-        <v>497</v>
-      </c>
-      <c r="C347" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="348" spans="2:3">
-      <c r="B348" t="s">
-        <v>498</v>
-      </c>
-      <c r="C348" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="349" spans="2:3">
-      <c r="B349" t="s">
-        <v>499</v>
-      </c>
-      <c r="C349" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="350" spans="2:3">
-      <c r="B350" t="s">
-        <v>500</v>
-      </c>
-      <c r="C350" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="351" spans="2:3">
-      <c r="B351" t="s">
-        <v>501</v>
-      </c>
-      <c r="C351" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="352" spans="2:3">
-      <c r="B352" t="s">
-        <v>502</v>
-      </c>
       <c r="C352" t="s">
-        <v>5</v>
+        <v>487</v>
       </c>
     </row>
     <row r="353" spans="2:3">
       <c r="B353" t="s">
-        <v>503</v>
+        <v>489</v>
       </c>
       <c r="C353" t="s">
-        <v>5</v>
+        <v>487</v>
       </c>
     </row>
     <row r="354" spans="2:3">
       <c r="B354" t="s">
-        <v>504</v>
+        <v>490</v>
       </c>
       <c r="C354" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="355" spans="2:3">
       <c r="B355" t="s">
-        <v>505</v>
+        <v>491</v>
       </c>
       <c r="C355" t="s">
-        <v>5</v>
+        <v>487</v>
       </c>
     </row>
     <row r="356" spans="2:3">
       <c r="B356" t="s">
-        <v>506</v>
+        <v>492</v>
       </c>
       <c r="C356" t="s">
-        <v>490</v>
+        <v>18</v>
       </c>
     </row>
     <row r="357" spans="2:3">
       <c r="B357" t="s">
-        <v>507</v>
+        <v>493</v>
       </c>
       <c r="C357" t="s">
-        <v>271</v>
+        <v>5</v>
       </c>
     </row>
     <row r="358" spans="2:3">
       <c r="B358" t="s">
-        <v>508</v>
+        <v>494</v>
       </c>
       <c r="C358" t="s">
         <v>5</v>
@@ -4715,239 +4842,224 @@
     </row>
     <row r="359" spans="2:3">
       <c r="B359" t="s">
-        <v>509</v>
+        <v>495</v>
       </c>
       <c r="C359" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="360" spans="2:3">
       <c r="B360" t="s">
-        <v>510</v>
+        <v>497</v>
       </c>
       <c r="C360" t="s">
-        <v>5</v>
+        <v>498</v>
       </c>
     </row>
     <row r="361" spans="2:3">
       <c r="B361" t="s">
-        <v>511</v>
+        <v>499</v>
       </c>
       <c r="C361" t="s">
-        <v>5</v>
+        <v>221</v>
       </c>
     </row>
     <row r="362" spans="2:3">
       <c r="B362" t="s">
-        <v>512</v>
+        <v>500</v>
       </c>
       <c r="C362" t="s">
-        <v>20</v>
+        <v>202</v>
       </c>
     </row>
     <row r="363" spans="2:3">
       <c r="B363" t="s">
-        <v>513</v>
+        <v>501</v>
       </c>
       <c r="C363" t="s">
-        <v>5</v>
+        <v>502</v>
       </c>
     </row>
     <row r="364" spans="2:3">
       <c r="B364" t="s">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="C364" t="s">
-        <v>5</v>
+        <v>312</v>
       </c>
     </row>
     <row r="365" spans="2:3">
       <c r="B365" t="s">
-        <v>515</v>
+        <v>504</v>
       </c>
       <c r="C365" t="s">
-        <v>483</v>
+        <v>505</v>
       </c>
     </row>
     <row r="366" spans="2:3">
       <c r="B366" t="s">
-        <v>516</v>
+        <v>506</v>
       </c>
       <c r="C366" t="s">
-        <v>5</v>
+        <v>117</v>
       </c>
     </row>
     <row r="367" spans="2:3">
       <c r="B367" t="s">
+        <v>507</v>
+      </c>
+      <c r="C367" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="369" spans="1:3">
+      <c r="A369" t="s">
+        <v>509</v>
+      </c>
+      <c r="B369" t="s">
+        <v>510</v>
+      </c>
+      <c r="C369" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="370" spans="1:3">
+      <c r="B370" t="s">
+        <v>512</v>
+      </c>
+      <c r="C370" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="371" spans="1:3">
+      <c r="B371" t="s">
+        <v>514</v>
+      </c>
+      <c r="C371" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="372" spans="1:3">
+      <c r="B372" t="s">
+        <v>515</v>
+      </c>
+      <c r="C372" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="373" spans="1:3">
+      <c r="B373" t="s">
+        <v>516</v>
+      </c>
+      <c r="C373" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="374" spans="1:3">
+      <c r="B374" t="s">
         <v>517</v>
       </c>
-      <c r="C367" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="368" spans="2:3">
-      <c r="B368" t="s">
+      <c r="C374" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="376" spans="1:3">
+      <c r="A376" t="s">
         <v>518</v>
       </c>
-      <c r="C368" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="369" spans="2:3">
-      <c r="B369" t="s">
+      <c r="B376" t="s">
         <v>519</v>
       </c>
-      <c r="C369" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="370" spans="2:3">
-      <c r="B370" t="s">
+      <c r="C376" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3">
+      <c r="A378" t="s">
         <v>520</v>
       </c>
-      <c r="C370" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="371" spans="2:3">
-      <c r="B371" t="s">
+      <c r="B378" t="s">
         <v>521</v>
       </c>
-      <c r="C371" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="372" spans="2:3">
-      <c r="B372" t="s">
+      <c r="C378" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="379" spans="1:3">
+      <c r="B379" t="s">
+        <v>198</v>
+      </c>
+      <c r="C379" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="380" spans="1:3">
+      <c r="B380" t="s">
         <v>522</v>
       </c>
-      <c r="C372" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="373" spans="2:3">
-      <c r="B373" t="s">
+      <c r="C380" t="s">
         <v>523</v>
       </c>
-      <c r="C373" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="374" spans="2:3">
-      <c r="B374" t="s">
+    </row>
+    <row r="381" spans="1:3">
+      <c r="B381" t="s">
         <v>524</v>
       </c>
-      <c r="C374" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="375" spans="2:3">
-      <c r="B375" t="s">
+      <c r="C381" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="382" spans="1:3">
+      <c r="B382" t="s">
         <v>525</v>
       </c>
-      <c r="C375" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="376" spans="2:3">
-      <c r="B376" t="s">
+      <c r="C382" t="s">
         <v>526</v>
       </c>
-      <c r="C376" t="s">
+    </row>
+    <row r="383" spans="1:3">
+      <c r="B383" t="s">
+        <v>527</v>
+      </c>
+      <c r="C383" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="377" spans="2:3">
-      <c r="B377" t="s">
-        <v>527</v>
-      </c>
-      <c r="C377" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="378" spans="2:3">
-      <c r="B378" t="s">
+    <row r="384" spans="1:3">
+      <c r="B384" t="s">
         <v>528</v>
       </c>
-      <c r="C378" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="379" spans="2:3">
-      <c r="B379" t="s">
+      <c r="C384" t="s">
         <v>529</v>
-      </c>
-      <c r="C379" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="380" spans="2:3">
-      <c r="B380" t="s">
-        <v>530</v>
-      </c>
-      <c r="C380" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="381" spans="2:3">
-      <c r="B381" t="s">
-        <v>531</v>
-      </c>
-      <c r="C381" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="382" spans="2:3">
-      <c r="B382" t="s">
-        <v>532</v>
-      </c>
-      <c r="C382" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="383" spans="2:3">
-      <c r="B383" t="s">
-        <v>533</v>
-      </c>
-      <c r="C383" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="384" spans="2:3">
-      <c r="B384" t="s">
-        <v>534</v>
-      </c>
-      <c r="C384" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="385" spans="2:3">
       <c r="B385" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="C385" t="s">
-        <v>463</v>
+        <v>18</v>
       </c>
     </row>
     <row r="386" spans="2:3">
       <c r="B386" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="C386" t="s">
-        <v>5</v>
+        <v>532</v>
       </c>
     </row>
     <row r="387" spans="2:3">
       <c r="B387" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="C387" t="s">
-        <v>495</v>
+        <v>534</v>
       </c>
     </row>
     <row r="388" spans="2:3">
       <c r="B388" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="C388" t="s">
         <v>5</v>
@@ -4955,7 +5067,7 @@
     </row>
     <row r="389" spans="2:3">
       <c r="B389" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C389" t="s">
         <v>5</v>
@@ -4963,7 +5075,7 @@
     </row>
     <row r="390" spans="2:3">
       <c r="B390" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="C390" t="s">
         <v>20</v>
@@ -4971,7 +5083,7 @@
     </row>
     <row r="391" spans="2:3">
       <c r="B391" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C391" t="s">
         <v>5</v>
@@ -4979,7 +5091,7 @@
     </row>
     <row r="392" spans="2:3">
       <c r="B392" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C392" t="s">
         <v>5</v>
@@ -4987,10 +5099,346 @@
     </row>
     <row r="393" spans="2:3">
       <c r="B393" t="s">
+        <v>540</v>
+      </c>
+      <c r="C393" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="394" spans="2:3">
+      <c r="B394" t="s">
+        <v>541</v>
+      </c>
+      <c r="C394" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="395" spans="2:3">
+      <c r="B395" t="s">
+        <v>542</v>
+      </c>
+      <c r="C395" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="396" spans="2:3">
+      <c r="B396" t="s">
         <v>543</v>
       </c>
-      <c r="C393" t="s">
+      <c r="C396" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="397" spans="2:3">
+      <c r="B397" t="s">
         <v>544</v>
+      </c>
+      <c r="C397" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="398" spans="2:3">
+      <c r="B398" t="s">
+        <v>545</v>
+      </c>
+      <c r="C398" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="399" spans="2:3">
+      <c r="B399" t="s">
+        <v>546</v>
+      </c>
+      <c r="C399" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="400" spans="2:3">
+      <c r="B400" t="s">
+        <v>547</v>
+      </c>
+      <c r="C400" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="401" spans="2:3">
+      <c r="B401" t="s">
+        <v>548</v>
+      </c>
+      <c r="C401" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="402" spans="2:3">
+      <c r="B402" t="s">
+        <v>549</v>
+      </c>
+      <c r="C402" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="403" spans="2:3">
+      <c r="B403" t="s">
+        <v>550</v>
+      </c>
+      <c r="C403" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="404" spans="2:3">
+      <c r="B404" t="s">
+        <v>551</v>
+      </c>
+      <c r="C404" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="405" spans="2:3">
+      <c r="B405" t="s">
+        <v>552</v>
+      </c>
+      <c r="C405" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="406" spans="2:3">
+      <c r="B406" t="s">
+        <v>553</v>
+      </c>
+      <c r="C406" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="407" spans="2:3">
+      <c r="B407" t="s">
+        <v>554</v>
+      </c>
+      <c r="C407" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="408" spans="2:3">
+      <c r="B408" t="s">
+        <v>555</v>
+      </c>
+      <c r="C408" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="409" spans="2:3">
+      <c r="B409" t="s">
+        <v>556</v>
+      </c>
+      <c r="C409" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="410" spans="2:3">
+      <c r="B410" t="s">
+        <v>557</v>
+      </c>
+      <c r="C410" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="411" spans="2:3">
+      <c r="B411" t="s">
+        <v>558</v>
+      </c>
+      <c r="C411" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="412" spans="2:3">
+      <c r="B412" t="s">
+        <v>559</v>
+      </c>
+      <c r="C412" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="413" spans="2:3">
+      <c r="B413" t="s">
+        <v>560</v>
+      </c>
+      <c r="C413" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="414" spans="2:3">
+      <c r="B414" t="s">
+        <v>561</v>
+      </c>
+      <c r="C414" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="415" spans="2:3">
+      <c r="B415" t="s">
+        <v>562</v>
+      </c>
+      <c r="C415" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="416" spans="2:3">
+      <c r="B416" t="s">
+        <v>563</v>
+      </c>
+      <c r="C416" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="417" spans="2:3">
+      <c r="B417" t="s">
+        <v>564</v>
+      </c>
+      <c r="C417" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="418" spans="2:3">
+      <c r="B418" t="s">
+        <v>565</v>
+      </c>
+      <c r="C418" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="419" spans="2:3">
+      <c r="B419" t="s">
+        <v>566</v>
+      </c>
+      <c r="C419" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="420" spans="2:3">
+      <c r="B420" t="s">
+        <v>567</v>
+      </c>
+      <c r="C420" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="421" spans="2:3">
+      <c r="B421" t="s">
+        <v>568</v>
+      </c>
+      <c r="C421" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="422" spans="2:3">
+      <c r="B422" t="s">
+        <v>569</v>
+      </c>
+      <c r="C422" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="423" spans="2:3">
+      <c r="B423" t="s">
+        <v>570</v>
+      </c>
+      <c r="C423" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="424" spans="2:3">
+      <c r="B424" t="s">
+        <v>571</v>
+      </c>
+      <c r="C424" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="425" spans="2:3">
+      <c r="B425" t="s">
+        <v>572</v>
+      </c>
+      <c r="C425" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="426" spans="2:3">
+      <c r="B426" t="s">
+        <v>573</v>
+      </c>
+      <c r="C426" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="427" spans="2:3">
+      <c r="B427" t="s">
+        <v>574</v>
+      </c>
+      <c r="C427" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="428" spans="2:3">
+      <c r="B428" t="s">
+        <v>575</v>
+      </c>
+      <c r="C428" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="429" spans="2:3">
+      <c r="B429" t="s">
+        <v>576</v>
+      </c>
+      <c r="C429" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="430" spans="2:3">
+      <c r="B430" t="s">
+        <v>577</v>
+      </c>
+      <c r="C430" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="431" spans="2:3">
+      <c r="B431" t="s">
+        <v>578</v>
+      </c>
+      <c r="C431" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="432" spans="2:3">
+      <c r="B432" t="s">
+        <v>579</v>
+      </c>
+      <c r="C432" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="433" spans="2:3">
+      <c r="B433" t="s">
+        <v>580</v>
+      </c>
+      <c r="C433" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="434" spans="2:3">
+      <c r="B434" t="s">
+        <v>581</v>
+      </c>
+      <c r="C434" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="435" spans="2:3">
+      <c r="B435" t="s">
+        <v>582</v>
+      </c>
+      <c r="C435" t="s">
+        <v>583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
files for pysam 7.1.0
</commit_message>
<xml_diff>
--- a/Examples/SelectingModuleandInverterExample/pySAM_Pvsamv1_default_values.xlsx
+++ b/Examples/SelectingModuleandInverterExample/pySAM_Pvsamv1_default_values.xlsx
@@ -14,33 +14,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="598">
   <si>
     <t>AdjustmentFactors</t>
   </si>
   <si>
-    <t>constant</t>
+    <t>adjust_constant</t>
   </si>
   <si>
     <t>0.0</t>
   </si>
   <si>
-    <t>en_periods</t>
-  </si>
-  <si>
-    <t>en_timeindex</t>
-  </si>
-  <si>
-    <t>periods</t>
+    <t>adjust_en_periods</t>
+  </si>
+  <si>
+    <t>adjust_en_timeindex</t>
+  </si>
+  <si>
+    <t>adjust_periods</t>
   </si>
   <si>
     <t>((0.0, 0.0, 0.0),)</t>
   </si>
   <si>
-    <t>timeindex</t>
+    <t>adjust_timeindex</t>
   </si>
   <si>
     <t>(0.0,)</t>
+  </si>
+  <si>
+    <t>dc_adjust_constant</t>
+  </si>
+  <si>
+    <t>dc_adjust_en_periods</t>
+  </si>
+  <si>
+    <t>dc_adjust_en_timeindex</t>
+  </si>
+  <si>
+    <t>dc_adjust_periods</t>
+  </si>
+  <si>
+    <t>dc_adjust_timeindex</t>
   </si>
   <si>
     <t>BatteryCell</t>
@@ -2124,7 +2139,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C443"/>
+  <dimension ref="A2:C448"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2173,335 +2188,335 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7" spans="1:3">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>9</v>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>10</v>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="B13" t="s">
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="B14" t="s">
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B17" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="B15" t="s">
+      <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="18" spans="1:3">
+      <c r="B18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="B16" t="s">
+      <c r="C18" t="s">
         <v>22</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" t="s">
+      <c r="C19" t="s">
         <v>24</v>
       </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18" t="s">
+      <c r="C20" t="s">
         <v>26</v>
       </c>
-      <c r="C18" t="s">
+    </row>
+    <row r="21" spans="1:3">
+      <c r="B21" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="B19" t="s">
+      <c r="C21" t="s">
         <v>28</v>
       </c>
-      <c r="C19" t="s">
+    </row>
+    <row r="22" spans="1:3">
+      <c r="B22" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="B20" t="s">
+      <c r="C22" t="s">
         <v>30</v>
       </c>
-      <c r="C20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3">
-      <c r="B21" t="s">
+    </row>
+    <row r="23" spans="1:3">
+      <c r="B23" t="s">
         <v>31</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
-      <c r="B22" t="s">
+    <row r="24" spans="1:3">
+      <c r="B24" t="s">
         <v>33</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
-      <c r="B23" t="s">
+    <row r="25" spans="1:3">
+      <c r="B25" t="s">
         <v>35</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="B26" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="2:3">
-      <c r="B24" t="s">
+      <c r="C26" t="s">
         <v>37</v>
       </c>
-      <c r="C24" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3">
-      <c r="B25" t="s">
+    </row>
+    <row r="27" spans="1:3">
+      <c r="B27" t="s">
         <v>38</v>
       </c>
-      <c r="C25" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3">
-      <c r="B26" t="s">
+      <c r="C27" t="s">
         <v>39</v>
       </c>
-      <c r="C26" t="s">
+    </row>
+    <row r="28" spans="1:3">
+      <c r="B28" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="2:3">
-      <c r="B27" t="s">
+      <c r="C28" t="s">
         <v>41</v>
       </c>
-      <c r="C27" t="s">
+    </row>
+    <row r="29" spans="1:3">
+      <c r="B29" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" spans="2:3">
-      <c r="B28" t="s">
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="B30" t="s">
         <v>43</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="B31" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="29" spans="2:3">
-      <c r="B29" t="s">
+      <c r="C31" t="s">
         <v>45</v>
       </c>
-      <c r="C29" t="s">
+    </row>
+    <row r="32" spans="1:3">
+      <c r="B32" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="30" spans="2:3">
-      <c r="B30" t="s">
+      <c r="C32" t="s">
         <v>47</v>
       </c>
-      <c r="C30" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3">
-      <c r="B31" t="s">
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" t="s">
         <v>48</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="2:3">
-      <c r="B32" t="s">
+    <row r="34" spans="2:3">
+      <c r="B34" t="s">
         <v>50</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C34" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="B33" t="s">
+    <row r="35" spans="2:3">
+      <c r="B35" t="s">
         <v>52</v>
       </c>
-      <c r="C33" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="B34" t="s">
+      <c r="C35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3">
+      <c r="B36" t="s">
         <v>53</v>
       </c>
-      <c r="C34" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="B35" t="s">
+      <c r="C36" t="s">
         <v>54</v>
       </c>
-      <c r="C35" t="s">
+    </row>
+    <row r="37" spans="2:3">
+      <c r="B37" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="B36" t="s">
+      <c r="C37" t="s">
         <v>56</v>
       </c>
-      <c r="C36" t="s">
+    </row>
+    <row r="38" spans="2:3">
+      <c r="B38" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="B37" t="s">
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
+      <c r="B39" t="s">
         <v>58</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="B38" t="s">
+      <c r="C40" t="s">
         <v>60</v>
       </c>
-      <c r="C38" t="s">
+    </row>
+    <row r="41" spans="2:3">
+      <c r="B41" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="B39" t="s">
+      <c r="C41" t="s">
         <v>62</v>
       </c>
-      <c r="C39" t="s">
+    </row>
+    <row r="42" spans="2:3">
+      <c r="B42" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="B40" t="s">
+      <c r="C42" t="s">
         <v>64</v>
       </c>
-      <c r="C40" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="B41" t="s">
+    </row>
+    <row r="43" spans="2:3">
+      <c r="B43" t="s">
         <v>65</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C43" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
-      <c r="B42" t="s">
+    <row r="44" spans="2:3">
+      <c r="B44" t="s">
         <v>67</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C44" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
-      <c r="B43" t="s">
+    <row r="45" spans="2:3">
+      <c r="B45" t="s">
         <v>69</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3">
+      <c r="B46" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
+      <c r="C46" t="s">
         <v>71</v>
       </c>
-      <c r="B45" t="s">
+    </row>
+    <row r="47" spans="2:3">
+      <c r="B47" t="s">
         <v>72</v>
       </c>
-      <c r="C45" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="B46" t="s">
+      <c r="C47" t="s">
         <v>73</v>
       </c>
-      <c r="C46" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="B47" t="s">
+    </row>
+    <row r="48" spans="2:3">
+      <c r="B48" t="s">
         <v>74</v>
       </c>
-      <c r="C47" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>75</v>
       </c>
-      <c r="C48" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="B49" t="s">
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
         <v>76</v>
       </c>
-      <c r="C49" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
       <c r="B50" t="s">
         <v>77</v>
       </c>
       <c r="C50" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -2509,7 +2524,7 @@
         <v>78</v>
       </c>
       <c r="C51" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -2517,36 +2532,36 @@
         <v>79</v>
       </c>
       <c r="C52" t="s">
-        <v>80</v>
+        <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="B53" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C53" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="B54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C54" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="B55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C55" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="B56" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C56" t="s">
         <v>2</v>
@@ -2554,10 +2569,10 @@
     </row>
     <row r="57" spans="1:3">
       <c r="B57" t="s">
+        <v>84</v>
+      </c>
+      <c r="C57" t="s">
         <v>85</v>
-      </c>
-      <c r="C57" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -2565,7 +2580,7 @@
         <v>86</v>
       </c>
       <c r="C58" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -2573,7 +2588,7 @@
         <v>87</v>
       </c>
       <c r="C59" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -2581,7 +2596,7 @@
         <v>88</v>
       </c>
       <c r="C60" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -2589,7 +2604,7 @@
         <v>89</v>
       </c>
       <c r="C61" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -2597,205 +2612,205 @@
         <v>90</v>
       </c>
       <c r="C62" t="s">
-        <v>70</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="B63" t="s">
+        <v>91</v>
+      </c>
+      <c r="C63" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" t="s">
-        <v>91</v>
-      </c>
       <c r="B64" t="s">
         <v>92</v>
       </c>
       <c r="C64" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
       <c r="B65" t="s">
         <v>93</v>
       </c>
       <c r="C65" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="B66" t="s">
         <v>94</v>
       </c>
       <c r="C66" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="B67" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="67" spans="2:3">
-      <c r="B67" t="s">
+      <c r="C67" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
         <v>96</v>
       </c>
-      <c r="C67" t="s">
+      <c r="B69" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="68" spans="2:3">
-      <c r="B68" t="s">
+      <c r="C69" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="B70" t="s">
         <v>98</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C70" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="B71" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="69" spans="2:3">
-      <c r="B69" t="s">
+      <c r="C71" t="s">
         <v>100</v>
       </c>
-      <c r="C69" t="s">
+    </row>
+    <row r="72" spans="1:3">
+      <c r="B72" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="70" spans="2:3">
-      <c r="B70" t="s">
+      <c r="C72" t="s">
         <v>102</v>
       </c>
-      <c r="C70" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3">
-      <c r="B71" t="s">
+    </row>
+    <row r="73" spans="1:3">
+      <c r="B73" t="s">
         <v>103</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C73" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="72" spans="2:3">
-      <c r="B72" t="s">
+    <row r="74" spans="1:3">
+      <c r="B74" t="s">
         <v>105</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C74" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="73" spans="2:3">
-      <c r="B73" t="s">
+    <row r="75" spans="1:3">
+      <c r="B75" t="s">
         <v>107</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C75" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="B76" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="74" spans="2:3">
-      <c r="B74" t="s">
+      <c r="C76" t="s">
         <v>109</v>
       </c>
-      <c r="C74" t="s">
+    </row>
+    <row r="77" spans="1:3">
+      <c r="B77" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="75" spans="2:3">
-      <c r="B75" t="s">
+      <c r="C77" t="s">
         <v>111</v>
       </c>
-      <c r="C75" t="s">
+    </row>
+    <row r="78" spans="1:3">
+      <c r="B78" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="76" spans="2:3">
-      <c r="B76" t="s">
+      <c r="C78" t="s">
         <v>113</v>
       </c>
-      <c r="C76" t="s">
+    </row>
+    <row r="79" spans="1:3">
+      <c r="B79" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="77" spans="2:3">
-      <c r="B77" t="s">
+      <c r="C79" t="s">
         <v>115</v>
       </c>
-      <c r="C77" t="s">
+    </row>
+    <row r="80" spans="1:3">
+      <c r="B80" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="78" spans="2:3">
-      <c r="B78" t="s">
+      <c r="C80" t="s">
         <v>117</v>
       </c>
-      <c r="C78" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="2:3">
-      <c r="B79" t="s">
+    </row>
+    <row r="81" spans="2:3">
+      <c r="B81" t="s">
         <v>118</v>
       </c>
-      <c r="C79" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="2:3">
-      <c r="B80" t="s">
+      <c r="C81" t="s">
         <v>119</v>
       </c>
-      <c r="C80" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="B81" t="s">
+    </row>
+    <row r="82" spans="2:3">
+      <c r="B82" t="s">
         <v>120</v>
       </c>
-      <c r="C81" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="B82" t="s">
+      <c r="C82" t="s">
         <v>121</v>
       </c>
-      <c r="C82" t="s">
+    </row>
+    <row r="83" spans="2:3">
+      <c r="B83" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="B83" t="s">
+      <c r="C83" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3">
+      <c r="B84" t="s">
         <v>123</v>
       </c>
-      <c r="C83" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="B84" t="s">
+      <c r="C84" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3">
+      <c r="B85" t="s">
         <v>124</v>
       </c>
-      <c r="C84" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="B85" t="s">
+      <c r="C85" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3">
+      <c r="B86" t="s">
         <v>125</v>
       </c>
-      <c r="C85" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="B86" t="s">
+      <c r="C86" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3">
+      <c r="B87" t="s">
         <v>126</v>
       </c>
-      <c r="C86" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="B87" t="s">
+      <c r="C87" t="s">
         <v>127</v>
       </c>
-      <c r="C87" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
+    </row>
+    <row r="88" spans="2:3">
       <c r="B88" t="s">
         <v>128</v>
       </c>
@@ -2803,648 +2818,656 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="2:3">
       <c r="B89" t="s">
         <v>129</v>
       </c>
       <c r="C89" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3">
+      <c r="B90" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="B90" t="s">
+      <c r="C90" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3">
+      <c r="B91" t="s">
         <v>131</v>
       </c>
-      <c r="C90" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="B91" t="s">
+      <c r="C91" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3">
+      <c r="B92" t="s">
         <v>132</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C92" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3">
+      <c r="B93" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93" t="s">
+      <c r="C93" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3">
+      <c r="B94" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94" t="s">
+      <c r="C94" t="s">
         <v>135</v>
       </c>
-      <c r="B94" t="s">
+    </row>
+    <row r="95" spans="2:3">
+      <c r="B95" t="s">
         <v>136</v>
       </c>
-      <c r="C94" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="B95" t="s">
+      <c r="C95" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3">
+      <c r="B96" t="s">
         <v>137</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C96" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
-      <c r="B96" t="s">
-        <v>139</v>
-      </c>
-      <c r="C96" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B99" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C99" t="s">
-        <v>144</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="B100" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C100" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="B101" t="s">
+        <v>144</v>
+      </c>
+      <c r="C101" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
         <v>147</v>
       </c>
-      <c r="C101" t="s">
+      <c r="B104" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="B102" t="s">
+      <c r="C104" t="s">
         <v>149</v>
-      </c>
-      <c r="C102" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
-      <c r="B103" t="s">
-        <v>151</v>
-      </c>
-      <c r="C103" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="B104" t="s">
-        <v>153</v>
-      </c>
-      <c r="C104" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="B105" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C105" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="B106" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C106" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="B107" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C107" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="B108" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C108" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="B109" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C109" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="B110" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C110" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="B111" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C111" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="B112" t="s">
+        <v>164</v>
+      </c>
+      <c r="C112" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3">
+      <c r="B113" t="s">
+        <v>166</v>
+      </c>
+      <c r="C113" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3">
+      <c r="B114" t="s">
+        <v>168</v>
+      </c>
+      <c r="C114" t="s">
         <v>169</v>
       </c>
-      <c r="C112" t="s">
+    </row>
+    <row r="115" spans="2:3">
+      <c r="B115" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="113" spans="1:3">
-      <c r="B113" t="s">
+      <c r="C115" t="s">
         <v>171</v>
       </c>
-      <c r="C113" t="s">
+    </row>
+    <row r="116" spans="2:3">
+      <c r="B116" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="114" spans="1:3">
-      <c r="B114" t="s">
+      <c r="C116" t="s">
         <v>173</v>
       </c>
-      <c r="C114" t="s">
+    </row>
+    <row r="117" spans="2:3">
+      <c r="B117" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="115" spans="1:3">
-      <c r="B115" t="s">
+      <c r="C117" t="s">
         <v>175</v>
       </c>
-      <c r="C115" t="s">
+    </row>
+    <row r="118" spans="2:3">
+      <c r="B118" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="B116" t="s">
+      <c r="C118" t="s">
         <v>177</v>
       </c>
-      <c r="C116" t="s">
+    </row>
+    <row r="119" spans="2:3">
+      <c r="B119" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="117" spans="1:3">
-      <c r="B117" t="s">
+      <c r="C119" t="s">
         <v>179</v>
       </c>
-      <c r="C117" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3">
-      <c r="B118" t="s">
+    </row>
+    <row r="120" spans="2:3">
+      <c r="B120" t="s">
         <v>180</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C120" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
-      <c r="B119" t="s">
+    <row r="121" spans="2:3">
+      <c r="B121" t="s">
         <v>182</v>
       </c>
-      <c r="C119" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="B120" t="s">
+      <c r="C121" t="s">
         <v>183</v>
       </c>
-      <c r="C120" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3">
-      <c r="B121" t="s">
+    </row>
+    <row r="122" spans="2:3">
+      <c r="B122" t="s">
         <v>184</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C122" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3">
+      <c r="B123" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="B122" t="s">
+      <c r="C123" t="s">
         <v>186</v>
       </c>
-      <c r="C122" t="s">
+    </row>
+    <row r="124" spans="2:3">
+      <c r="B124" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="123" spans="1:3">
-      <c r="B123" t="s">
+      <c r="C124" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3">
+      <c r="B125" t="s">
         <v>188</v>
       </c>
-      <c r="C123" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3">
-      <c r="B124" t="s">
+      <c r="C125" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3">
+      <c r="B126" t="s">
         <v>189</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C126" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
-      <c r="A126" t="s">
+    <row r="127" spans="2:3">
+      <c r="B127" t="s">
         <v>191</v>
       </c>
-      <c r="B126" t="s">
+      <c r="C127" t="s">
         <v>192</v>
       </c>
-      <c r="C126" t="s">
+    </row>
+    <row r="128" spans="2:3">
+      <c r="B128" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="127" spans="1:3">
-      <c r="B127" t="s">
-        <v>194</v>
-      </c>
-      <c r="C127" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3">
-      <c r="B128" t="s">
-        <v>196</v>
-      </c>
       <c r="C128" t="s">
-        <v>187</v>
+        <v>66</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="B129" t="s">
+        <v>194</v>
+      </c>
+      <c r="C129" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" t="s">
+        <v>196</v>
+      </c>
+      <c r="B131" t="s">
         <v>197</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C131" t="s">
         <v>198</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3">
-      <c r="B130" t="s">
-        <v>199</v>
-      </c>
-      <c r="C130" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3">
-      <c r="B131" t="s">
-        <v>200</v>
-      </c>
-      <c r="C131" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="B132" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C132" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="B133" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C133" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="B134" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C134" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="B135" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C135" t="s">
-        <v>208</v>
+        <v>30</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="B136" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C136" t="s">
-        <v>2</v>
+        <v>206</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="B137" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C137" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="B138" t="s">
+        <v>208</v>
+      </c>
+      <c r="C138" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="B139" t="s">
+        <v>210</v>
+      </c>
+      <c r="C139" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="B140" t="s">
         <v>212</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C140" t="s">
         <v>213</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3">
-      <c r="A140" t="s">
-        <v>214</v>
-      </c>
-      <c r="B140" t="s">
-        <v>215</v>
-      </c>
-      <c r="C140" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="B141" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C141" t="s">
-        <v>218</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="B142" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C142" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="B143" t="s">
+        <v>217</v>
+      </c>
+      <c r="C143" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" t="s">
+        <v>219</v>
+      </c>
+      <c r="B145" t="s">
+        <v>220</v>
+      </c>
+      <c r="C145" t="s">
         <v>221</v>
-      </c>
-      <c r="C143" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3">
-      <c r="B144" t="s">
-        <v>194</v>
-      </c>
-      <c r="C144" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3">
-      <c r="B145" t="s">
-        <v>223</v>
-      </c>
-      <c r="C145" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="B146" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C146" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="B147" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C147" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="B148" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C148" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="B149" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="C149" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="B150" t="s">
+        <v>228</v>
+      </c>
+      <c r="C150" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="B151" t="s">
+        <v>230</v>
+      </c>
+      <c r="C151" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="B152" t="s">
+        <v>232</v>
+      </c>
+      <c r="C152" t="s">
         <v>233</v>
-      </c>
-      <c r="C150" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3">
-      <c r="A152" t="s">
-        <v>235</v>
-      </c>
-      <c r="B152" t="s">
-        <v>236</v>
-      </c>
-      <c r="C152" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="B153" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C153" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="B154" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C154" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="B155" t="s">
+        <v>238</v>
+      </c>
+      <c r="C155" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" t="s">
+        <v>240</v>
+      </c>
+      <c r="B157" t="s">
+        <v>241</v>
+      </c>
+      <c r="C157" t="s">
         <v>242</v>
-      </c>
-      <c r="C155" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3">
-      <c r="B156" t="s">
-        <v>205</v>
-      </c>
-      <c r="C156" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3">
-      <c r="B157" t="s">
-        <v>244</v>
-      </c>
-      <c r="C157" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="B158" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C158" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="B159" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C159" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="B160" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C160" t="s">
-        <v>211</v>
+        <v>248</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="B161" t="s">
-        <v>251</v>
+        <v>210</v>
       </c>
       <c r="C161" t="s">
-        <v>252</v>
+        <v>211</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="B162" t="s">
+        <v>249</v>
+      </c>
+      <c r="C162" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="B163" t="s">
+        <v>251</v>
+      </c>
+      <c r="C163" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="B164" t="s">
         <v>253</v>
       </c>
-      <c r="C162" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3">
-      <c r="A164" t="s">
+      <c r="C164" t="s">
         <v>254</v>
-      </c>
-      <c r="B164" t="s">
-        <v>196</v>
-      </c>
-      <c r="C164" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="B165" t="s">
-        <v>197</v>
+        <v>255</v>
       </c>
       <c r="C165" t="s">
-        <v>198</v>
+        <v>216</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="B166" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C166" t="s">
-        <v>25</v>
+        <v>257</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="B167" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C167" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3">
-      <c r="B168" t="s">
-        <v>257</v>
-      </c>
-      <c r="C168" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
     </row>
     <row r="169" spans="1:3">
+      <c r="A169" t="s">
+        <v>259</v>
+      </c>
       <c r="B169" t="s">
-        <v>258</v>
+        <v>201</v>
       </c>
       <c r="C169" t="s">
-        <v>259</v>
+        <v>192</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="B170" t="s">
+        <v>202</v>
+      </c>
+      <c r="C170" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="B171" t="s">
         <v>260</v>
       </c>
-      <c r="C170" t="s">
-        <v>234</v>
+      <c r="C171" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="172" spans="1:3">
-      <c r="A172" t="s">
+      <c r="B172" t="s">
         <v>261</v>
       </c>
+      <c r="C172" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="173" spans="1:3">
-      <c r="A173" t="s">
+      <c r="B173" t="s">
         <v>262</v>
       </c>
-      <c r="B173" t="s">
-        <v>263</v>
-      </c>
       <c r="C173" t="s">
-        <v>264</v>
+        <v>235</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="B174" t="s">
-        <v>202</v>
+        <v>263</v>
       </c>
       <c r="C174" t="s">
-        <v>198</v>
+        <v>264</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -3452,138 +3475,130 @@
         <v>265</v>
       </c>
       <c r="C175" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="176" spans="1:3">
-      <c r="B176" t="s">
+    <row r="178" spans="1:3">
+      <c r="A178" t="s">
         <v>267</v>
       </c>
-      <c r="C176" t="s">
+      <c r="B178" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="177" spans="1:3">
-      <c r="B177" t="s">
+      <c r="C178" t="s">
         <v>269</v>
-      </c>
-      <c r="C177" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3">
-      <c r="B178" t="s">
-        <v>270</v>
-      </c>
-      <c r="C178" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="B179" t="s">
-        <v>271</v>
+        <v>207</v>
       </c>
       <c r="C179" t="s">
-        <v>259</v>
+        <v>203</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="B180" t="s">
+        <v>270</v>
+      </c>
+      <c r="C180" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="B181" t="s">
         <v>272</v>
       </c>
-      <c r="C180" t="s">
-        <v>234</v>
+      <c r="C181" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="182" spans="1:3">
-      <c r="A182" t="s">
-        <v>273</v>
-      </c>
       <c r="B182" t="s">
         <v>274</v>
       </c>
       <c r="C182" t="s">
-        <v>275</v>
+        <v>2</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="B183" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C183" t="s">
-        <v>2</v>
+        <v>235</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="B184" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C184" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="B185" t="s">
+        <v>277</v>
+      </c>
+      <c r="C185" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" t="s">
+        <v>278</v>
+      </c>
+      <c r="B187" t="s">
         <v>279</v>
       </c>
-      <c r="C185" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3">
-      <c r="B186" t="s">
+      <c r="C187" t="s">
         <v>280</v>
-      </c>
-      <c r="C186" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3">
-      <c r="B187" t="s">
-        <v>281</v>
-      </c>
-      <c r="C187" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="B188" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C188" t="s">
-        <v>208</v>
+        <v>2</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="B189" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C189" t="s">
-        <v>2</v>
+        <v>283</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="B190" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C190" t="s">
-        <v>282</v>
+        <v>213</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="B191" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C191" t="s">
-        <v>208</v>
+        <v>2</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="B192" t="s">
+        <v>286</v>
+      </c>
+      <c r="C192" t="s">
         <v>287</v>
-      </c>
-      <c r="C192" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="193" spans="1:3">
@@ -3591,7 +3606,7 @@
         <v>288</v>
       </c>
       <c r="C193" t="s">
-        <v>282</v>
+        <v>213</v>
       </c>
     </row>
     <row r="194" spans="1:3">
@@ -3599,18 +3614,23 @@
         <v>289</v>
       </c>
       <c r="C194" t="s">
-        <v>208</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="B195" t="s">
+        <v>290</v>
+      </c>
+      <c r="C195" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="196" spans="1:3">
-      <c r="A196" t="s">
-        <v>290</v>
-      </c>
       <c r="B196" t="s">
         <v>291</v>
       </c>
       <c r="C196" t="s">
-        <v>130</v>
+        <v>213</v>
       </c>
     </row>
     <row r="197" spans="1:3">
@@ -3618,7 +3638,7 @@
         <v>292</v>
       </c>
       <c r="C197" t="s">
-        <v>278</v>
+        <v>2</v>
       </c>
     </row>
     <row r="198" spans="1:3">
@@ -3626,101 +3646,101 @@
         <v>293</v>
       </c>
       <c r="C198" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="B199" t="s">
+        <v>294</v>
+      </c>
+      <c r="C199" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" t="s">
         <v>295</v>
       </c>
-      <c r="C199" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3">
-      <c r="B200" t="s">
+      <c r="B201" t="s">
         <v>296</v>
       </c>
-      <c r="C200" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3">
-      <c r="B201" t="s">
-        <v>297</v>
-      </c>
       <c r="C201" t="s">
-        <v>2</v>
+        <v>135</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="B202" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C202" t="s">
-        <v>299</v>
+        <v>283</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="B203" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C203" t="s">
-        <v>25</v>
+        <v>299</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="B204" t="s">
+        <v>300</v>
+      </c>
+      <c r="C204" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="B205" t="s">
         <v>301</v>
       </c>
-      <c r="C204" t="s">
-        <v>25</v>
+      <c r="C205" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="206" spans="1:3">
-      <c r="A206" t="s">
+      <c r="B206" t="s">
         <v>302</v>
       </c>
-      <c r="B206" t="s">
-        <v>303</v>
-      </c>
       <c r="C206" t="s">
-        <v>304</v>
+        <v>2</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="B207" t="s">
+        <v>303</v>
+      </c>
+      <c r="C207" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="B208" t="s">
         <v>305</v>
       </c>
-      <c r="C207" t="s">
-        <v>8</v>
+      <c r="C208" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="209" spans="1:3">
-      <c r="A209" t="s">
+      <c r="B209" t="s">
         <v>306</v>
       </c>
-      <c r="B209" t="s">
+      <c r="C209" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211" t="s">
         <v>307</v>
       </c>
-      <c r="C209" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3">
-      <c r="B210" t="s">
+      <c r="B211" t="s">
         <v>308</v>
       </c>
-      <c r="C210" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3">
-      <c r="B211" t="s">
+      <c r="C211" t="s">
         <v>309</v>
-      </c>
-      <c r="C211" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="212" spans="1:3">
@@ -3728,23 +3748,18 @@
         <v>310</v>
       </c>
       <c r="C212" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3">
-      <c r="B213" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
+      <c r="A214" t="s">
         <v>311</v>
       </c>
-      <c r="C213" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3">
       <c r="B214" t="s">
         <v>312</v>
       </c>
       <c r="C214" t="s">
-        <v>208</v>
+        <v>30</v>
       </c>
     </row>
     <row r="215" spans="1:3">
@@ -3752,12 +3767,12 @@
         <v>313</v>
       </c>
       <c r="C215" t="s">
-        <v>314</v>
+        <v>30</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="B216" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C216" t="s">
         <v>2</v>
@@ -3765,15 +3780,15 @@
     </row>
     <row r="217" spans="1:3">
       <c r="B217" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C217" t="s">
-        <v>208</v>
+        <v>2</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="B218" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C218" t="s">
         <v>2</v>
@@ -3781,55 +3796,55 @@
     </row>
     <row r="219" spans="1:3">
       <c r="B219" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C219" t="s">
-        <v>319</v>
+        <v>213</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="B220" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C220" t="s">
-        <v>2</v>
+        <v>319</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="B221" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C221" t="s">
-        <v>322</v>
+        <v>2</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="B222" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C222" t="s">
-        <v>2</v>
+        <v>213</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="B223" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C223" t="s">
-        <v>208</v>
+        <v>2</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="B224" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C224" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
     </row>
     <row r="225" spans="2:3">
       <c r="B225" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C225" t="s">
         <v>2</v>
@@ -3837,10 +3852,10 @@
     </row>
     <row r="226" spans="2:3">
       <c r="B226" t="s">
+        <v>326</v>
+      </c>
+      <c r="C226" t="s">
         <v>327</v>
-      </c>
-      <c r="C226" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="227" spans="2:3">
@@ -3856,7 +3871,7 @@
         <v>329</v>
       </c>
       <c r="C228" t="s">
-        <v>2</v>
+        <v>213</v>
       </c>
     </row>
     <row r="229" spans="2:3">
@@ -3864,7 +3879,7 @@
         <v>330</v>
       </c>
       <c r="C229" t="s">
-        <v>2</v>
+        <v>319</v>
       </c>
     </row>
     <row r="230" spans="2:3">
@@ -3872,7 +3887,7 @@
         <v>331</v>
       </c>
       <c r="C230" t="s">
-        <v>322</v>
+        <v>2</v>
       </c>
     </row>
     <row r="231" spans="2:3">
@@ -3880,7 +3895,7 @@
         <v>332</v>
       </c>
       <c r="C231" t="s">
-        <v>2</v>
+        <v>213</v>
       </c>
     </row>
     <row r="232" spans="2:3">
@@ -3888,7 +3903,7 @@
         <v>333</v>
       </c>
       <c r="C232" t="s">
-        <v>208</v>
+        <v>2</v>
       </c>
     </row>
     <row r="233" spans="2:3">
@@ -3896,7 +3911,7 @@
         <v>334</v>
       </c>
       <c r="C233" t="s">
-        <v>314</v>
+        <v>2</v>
       </c>
     </row>
     <row r="234" spans="2:3">
@@ -3912,7 +3927,7 @@
         <v>336</v>
       </c>
       <c r="C235" t="s">
-        <v>208</v>
+        <v>327</v>
       </c>
     </row>
     <row r="236" spans="2:3">
@@ -3928,7 +3943,7 @@
         <v>338</v>
       </c>
       <c r="C237" t="s">
-        <v>2</v>
+        <v>213</v>
       </c>
     </row>
     <row r="238" spans="2:3">
@@ -3936,7 +3951,7 @@
         <v>339</v>
       </c>
       <c r="C238" t="s">
-        <v>2</v>
+        <v>319</v>
       </c>
     </row>
     <row r="239" spans="2:3">
@@ -3944,7 +3959,7 @@
         <v>340</v>
       </c>
       <c r="C239" t="s">
-        <v>322</v>
+        <v>2</v>
       </c>
     </row>
     <row r="240" spans="2:3">
@@ -3952,26 +3967,26 @@
         <v>341</v>
       </c>
       <c r="C240" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="241" spans="2:3">
       <c r="B241" t="s">
         <v>342</v>
       </c>
       <c r="C241" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="242" spans="2:3">
       <c r="B242" t="s">
         <v>343</v>
       </c>
       <c r="C242" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="243" spans="2:3">
       <c r="B243" t="s">
         <v>344</v>
       </c>
@@ -3979,15 +3994,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="244" spans="1:3">
+    <row r="244" spans="2:3">
       <c r="B244" t="s">
         <v>345</v>
       </c>
       <c r="C244" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="245" spans="2:3">
       <c r="B245" t="s">
         <v>346</v>
       </c>
@@ -3995,39 +4010,39 @@
         <v>2</v>
       </c>
     </row>
-    <row r="246" spans="1:3">
+    <row r="246" spans="2:3">
       <c r="B246" t="s">
         <v>347</v>
       </c>
       <c r="C246" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="247" spans="2:3">
       <c r="B247" t="s">
         <v>348</v>
       </c>
       <c r="C247" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="248" spans="2:3">
       <c r="B248" t="s">
         <v>349</v>
       </c>
       <c r="C248" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="249" spans="2:3">
       <c r="B249" t="s">
         <v>350</v>
       </c>
       <c r="C249" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="250" spans="1:3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="250" spans="2:3">
       <c r="B250" t="s">
         <v>351</v>
       </c>
@@ -4035,7 +4050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="251" spans="1:3">
+    <row r="251" spans="2:3">
       <c r="B251" t="s">
         <v>352</v>
       </c>
@@ -4043,7 +4058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="252" spans="1:3">
+    <row r="252" spans="2:3">
       <c r="B252" t="s">
         <v>353</v>
       </c>
@@ -4051,49 +4066,60 @@
         <v>2</v>
       </c>
     </row>
-    <row r="254" spans="1:3">
-      <c r="A254" t="s">
+    <row r="253" spans="2:3">
+      <c r="B253" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="255" spans="1:3">
-      <c r="A255" t="s">
+      <c r="C253" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="254" spans="2:3">
+      <c r="B254" t="s">
         <v>355</v>
       </c>
+      <c r="C254" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="255" spans="2:3">
       <c r="B255" t="s">
         <v>356</v>
       </c>
       <c r="C255" t="s">
-        <v>25</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="256" spans="2:3">
+      <c r="B256" t="s">
+        <v>357</v>
+      </c>
+      <c r="C256" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="257" spans="1:3">
-      <c r="A257" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3">
-      <c r="A258" t="s">
+      <c r="B257" t="s">
         <v>358</v>
       </c>
-      <c r="B258" t="s">
+      <c r="C257" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3">
+      <c r="A259" t="s">
         <v>359</v>
       </c>
-      <c r="C258" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3">
-      <c r="B259" t="s">
+    </row>
+    <row r="260" spans="1:3">
+      <c r="A260" t="s">
         <v>360</v>
       </c>
-      <c r="C259" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="261" spans="1:3">
-      <c r="A261" t="s">
+      <c r="B260" t="s">
         <v>361</v>
+      </c>
+      <c r="C260" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="262" spans="1:3">
@@ -4109,327 +4135,316 @@
         <v>364</v>
       </c>
       <c r="C263" t="s">
-        <v>365</v>
+        <v>2</v>
       </c>
     </row>
     <row r="264" spans="1:3">
       <c r="B264" t="s">
+        <v>365</v>
+      </c>
+      <c r="C264" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3">
+      <c r="A266" t="s">
         <v>366</v>
       </c>
-      <c r="C264" t="s">
+    </row>
+    <row r="267" spans="1:3">
+      <c r="A267" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="265" spans="1:3">
-      <c r="B265" t="s">
+    <row r="268" spans="1:3">
+      <c r="A268" t="s">
         <v>368</v>
       </c>
-      <c r="C265" t="s">
+      <c r="B268" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="266" spans="1:3">
-      <c r="B266" t="s">
+      <c r="C268" t="s">
         <v>370</v>
-      </c>
-      <c r="C266" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="267" spans="1:3">
-      <c r="B267" t="s">
-        <v>372</v>
-      </c>
-      <c r="C267" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="268" spans="1:3">
-      <c r="B268" t="s">
-        <v>374</v>
-      </c>
-      <c r="C268" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="269" spans="1:3">
       <c r="B269" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C269" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="270" spans="1:3">
       <c r="B270" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="C270" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
     <row r="271" spans="1:3">
       <c r="B271" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="C271" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="272" spans="1:3">
       <c r="B272" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="C272" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="273" spans="2:3">
       <c r="B273" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C273" t="s">
-        <v>25</v>
+        <v>380</v>
       </c>
     </row>
     <row r="274" spans="2:3">
       <c r="B274" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C274" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="275" spans="2:3">
       <c r="B275" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="C275" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="276" spans="2:3">
       <c r="B276" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="C276" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="277" spans="2:3">
       <c r="B277" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="C277" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="278" spans="2:3">
       <c r="B278" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C278" t="s">
-        <v>394</v>
+        <v>30</v>
       </c>
     </row>
     <row r="279" spans="2:3">
       <c r="B279" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="C279" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="280" spans="2:3">
       <c r="B280" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="C280" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="281" spans="2:3">
       <c r="B281" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="C281" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="282" spans="2:3">
       <c r="B282" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="C282" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
     </row>
     <row r="283" spans="2:3">
       <c r="B283" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="C283" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
     </row>
     <row r="284" spans="2:3">
       <c r="B284" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="C284" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="285" spans="2:3">
       <c r="B285" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C285" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
     </row>
     <row r="286" spans="2:3">
       <c r="B286" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="C286" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="287" spans="2:3">
       <c r="B287" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="C287" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="288" spans="2:3">
       <c r="B288" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="C288" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="289" spans="2:3">
       <c r="B289" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="C289" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="290" spans="2:3">
       <c r="B290" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="C290" t="s">
-        <v>25</v>
+        <v>413</v>
       </c>
     </row>
     <row r="291" spans="2:3">
       <c r="B291" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="C291" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="292" spans="2:3">
       <c r="B292" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C292" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="293" spans="2:3">
       <c r="B293" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="C293" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="294" spans="2:3">
       <c r="B294" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C294" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="295" spans="2:3">
       <c r="B295" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C295" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="296" spans="2:3">
       <c r="B296" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C296" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
     </row>
     <row r="297" spans="2:3">
       <c r="B297" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C297" t="s">
-        <v>2</v>
+        <v>426</v>
       </c>
     </row>
     <row r="298" spans="2:3">
       <c r="B298" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C298" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="299" spans="2:3">
       <c r="B299" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C299" t="s">
-        <v>365</v>
+        <v>430</v>
       </c>
     </row>
     <row r="300" spans="2:3">
       <c r="B300" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C300" t="s">
-        <v>383</v>
+        <v>2</v>
       </c>
     </row>
     <row r="301" spans="2:3">
       <c r="B301" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C301" t="s">
-        <v>416</v>
+        <v>2</v>
       </c>
     </row>
     <row r="302" spans="2:3">
       <c r="B302" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C302" t="s">
-        <v>187</v>
+        <v>2</v>
       </c>
     </row>
     <row r="303" spans="2:3">
       <c r="B303" t="s">
+        <v>434</v>
+      </c>
+      <c r="C303" t="s">
         <v>435</v>
-      </c>
-      <c r="C303" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="304" spans="2:3">
@@ -4437,63 +4452,63 @@
         <v>436</v>
       </c>
       <c r="C304" t="s">
-        <v>437</v>
+        <v>370</v>
       </c>
     </row>
     <row r="305" spans="1:3">
       <c r="B305" t="s">
+        <v>437</v>
+      </c>
+      <c r="C305" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3">
+      <c r="B306" t="s">
         <v>438</v>
       </c>
-      <c r="C305" t="s">
+      <c r="C306" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3">
+      <c r="B307" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="307" spans="1:3">
-      <c r="A307" t="s">
-        <v>440</v>
-      </c>
-      <c r="B307" t="s">
-        <v>441</v>
-      </c>
       <c r="C307" t="s">
-        <v>2</v>
+        <v>192</v>
       </c>
     </row>
     <row r="308" spans="1:3">
       <c r="B308" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C308" t="s">
-        <v>443</v>
+        <v>71</v>
       </c>
     </row>
     <row r="309" spans="1:3">
       <c r="B309" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C309" t="s">
-        <v>2</v>
+        <v>442</v>
       </c>
     </row>
     <row r="310" spans="1:3">
       <c r="B310" t="s">
+        <v>443</v>
+      </c>
+      <c r="C310" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3">
+      <c r="A312" t="s">
         <v>445</v>
       </c>
-      <c r="C310" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="311" spans="1:3">
-      <c r="B311" t="s">
+      <c r="B312" t="s">
         <v>446</v>
-      </c>
-      <c r="C311" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="312" spans="1:3">
-      <c r="B312" t="s">
-        <v>447</v>
       </c>
       <c r="C312" t="s">
         <v>2</v>
@@ -4501,10 +4516,10 @@
     </row>
     <row r="313" spans="1:3">
       <c r="B313" t="s">
+        <v>447</v>
+      </c>
+      <c r="C313" t="s">
         <v>448</v>
-      </c>
-      <c r="C313" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="314" spans="1:3">
@@ -4520,7 +4535,7 @@
         <v>450</v>
       </c>
       <c r="C315" t="s">
-        <v>443</v>
+        <v>2</v>
       </c>
     </row>
     <row r="316" spans="1:3">
@@ -4536,7 +4551,7 @@
         <v>452</v>
       </c>
       <c r="C317" t="s">
-        <v>443</v>
+        <v>2</v>
       </c>
     </row>
     <row r="318" spans="1:3">
@@ -4552,7 +4567,7 @@
         <v>454</v>
       </c>
       <c r="C319" t="s">
-        <v>443</v>
+        <v>2</v>
       </c>
     </row>
     <row r="320" spans="1:3">
@@ -4560,7 +4575,7 @@
         <v>455</v>
       </c>
       <c r="C320" t="s">
-        <v>2</v>
+        <v>448</v>
       </c>
     </row>
     <row r="321" spans="2:3">
@@ -4576,7 +4591,7 @@
         <v>457</v>
       </c>
       <c r="C322" t="s">
-        <v>2</v>
+        <v>448</v>
       </c>
     </row>
     <row r="323" spans="2:3">
@@ -4592,7 +4607,7 @@
         <v>459</v>
       </c>
       <c r="C324" t="s">
-        <v>2</v>
+        <v>448</v>
       </c>
     </row>
     <row r="325" spans="2:3">
@@ -4608,7 +4623,7 @@
         <v>461</v>
       </c>
       <c r="C326" t="s">
-        <v>443</v>
+        <v>2</v>
       </c>
     </row>
     <row r="327" spans="2:3">
@@ -4624,7 +4639,7 @@
         <v>463</v>
       </c>
       <c r="C328" t="s">
-        <v>443</v>
+        <v>2</v>
       </c>
     </row>
     <row r="329" spans="2:3">
@@ -4640,7 +4655,7 @@
         <v>465</v>
       </c>
       <c r="C330" t="s">
-        <v>443</v>
+        <v>2</v>
       </c>
     </row>
     <row r="331" spans="2:3">
@@ -4648,7 +4663,7 @@
         <v>466</v>
       </c>
       <c r="C331" t="s">
-        <v>2</v>
+        <v>448</v>
       </c>
     </row>
     <row r="332" spans="2:3">
@@ -4664,7 +4679,7 @@
         <v>468</v>
       </c>
       <c r="C333" t="s">
-        <v>2</v>
+        <v>448</v>
       </c>
     </row>
     <row r="334" spans="2:3">
@@ -4680,7 +4695,7 @@
         <v>470</v>
       </c>
       <c r="C335" t="s">
-        <v>2</v>
+        <v>448</v>
       </c>
     </row>
     <row r="336" spans="2:3">
@@ -4691,15 +4706,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="337" spans="1:3">
+    <row r="337" spans="2:3">
       <c r="B337" t="s">
         <v>472</v>
       </c>
       <c r="C337" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="338" spans="1:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="338" spans="2:3">
       <c r="B338" t="s">
         <v>473</v>
       </c>
@@ -4707,15 +4722,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="339" spans="1:3">
+    <row r="339" spans="2:3">
       <c r="B339" t="s">
         <v>474</v>
       </c>
       <c r="C339" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="340" spans="1:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="340" spans="2:3">
       <c r="B340" t="s">
         <v>475</v>
       </c>
@@ -4723,23 +4738,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="341" spans="1:3">
+    <row r="341" spans="2:3">
       <c r="B341" t="s">
         <v>476</v>
       </c>
       <c r="C341" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="342" spans="1:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="342" spans="2:3">
       <c r="B342" t="s">
         <v>477</v>
       </c>
       <c r="C342" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="343" spans="1:3">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="343" spans="2:3">
       <c r="B343" t="s">
         <v>478</v>
       </c>
@@ -4747,15 +4762,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="344" spans="1:3">
+    <row r="344" spans="2:3">
       <c r="B344" t="s">
         <v>479</v>
       </c>
       <c r="C344" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="345" spans="1:3">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="345" spans="2:3">
       <c r="B345" t="s">
         <v>480</v>
       </c>
@@ -4763,15 +4778,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="346" spans="1:3">
+    <row r="346" spans="2:3">
       <c r="B346" t="s">
         <v>481</v>
       </c>
       <c r="C346" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="347" spans="1:3">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="347" spans="2:3">
       <c r="B347" t="s">
         <v>482</v>
       </c>
@@ -4779,15 +4794,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="348" spans="1:3">
+    <row r="348" spans="2:3">
       <c r="B348" t="s">
         <v>483</v>
       </c>
       <c r="C348" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="349" spans="1:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="349" spans="2:3">
       <c r="B349" t="s">
         <v>484</v>
       </c>
@@ -4795,264 +4810,269 @@
         <v>2</v>
       </c>
     </row>
-    <row r="350" spans="1:3">
+    <row r="350" spans="2:3">
       <c r="B350" t="s">
         <v>485</v>
       </c>
       <c r="C350" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="352" spans="1:3">
-      <c r="A352" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="351" spans="2:3">
+      <c r="B351" t="s">
         <v>486</v>
       </c>
+      <c r="C351" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="352" spans="2:3">
       <c r="B352" t="s">
         <v>487</v>
       </c>
       <c r="C352" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3">
+      <c r="B353" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="353" spans="2:3">
-      <c r="B353" t="s">
+      <c r="C353" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3">
+      <c r="B354" t="s">
         <v>489</v>
       </c>
-      <c r="C353" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="354" spans="2:3">
-      <c r="B354" t="s">
+      <c r="C354" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3">
+      <c r="B355" t="s">
         <v>490</v>
       </c>
-      <c r="C354" t="s">
+      <c r="C355" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3">
+      <c r="A357" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="355" spans="2:3">
-      <c r="B355" t="s">
+      <c r="B357" t="s">
         <v>492</v>
       </c>
-      <c r="C355" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="356" spans="2:3">
-      <c r="B356" t="s">
+      <c r="C357" t="s">
         <v>493</v>
       </c>
-      <c r="C356" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="357" spans="2:3">
-      <c r="B357" t="s">
+    </row>
+    <row r="358" spans="1:3">
+      <c r="B358" t="s">
         <v>494</v>
       </c>
-      <c r="C357" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="358" spans="2:3">
-      <c r="B358" t="s">
+      <c r="C358" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3">
+      <c r="B359" t="s">
         <v>495</v>
       </c>
-      <c r="C358" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="359" spans="2:3">
-      <c r="B359" t="s">
+      <c r="C359" t="s">
         <v>496</v>
       </c>
-      <c r="C359" t="s">
+    </row>
+    <row r="360" spans="1:3">
+      <c r="B360" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="360" spans="2:3">
-      <c r="B360" t="s">
+      <c r="C360" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3">
+      <c r="B361" t="s">
         <v>498</v>
       </c>
-      <c r="C360" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="361" spans="2:3">
-      <c r="B361" t="s">
+      <c r="C361" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3">
+      <c r="B362" t="s">
         <v>499</v>
       </c>
-      <c r="C361" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="362" spans="2:3">
-      <c r="B362" t="s">
+      <c r="C362" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3">
+      <c r="B363" t="s">
         <v>500</v>
       </c>
-      <c r="C362" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="363" spans="2:3">
-      <c r="B363" t="s">
+      <c r="C363" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="364" spans="1:3">
+      <c r="B364" t="s">
         <v>501</v>
       </c>
-      <c r="C363" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="364" spans="2:3">
-      <c r="B364" t="s">
+      <c r="C364" t="s">
         <v>502</v>
       </c>
-      <c r="C364" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="365" spans="2:3">
+    </row>
+    <row r="365" spans="1:3">
       <c r="B365" t="s">
         <v>503</v>
       </c>
       <c r="C365" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="366" spans="2:3">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="366" spans="1:3">
       <c r="B366" t="s">
         <v>504</v>
       </c>
       <c r="C366" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="367" spans="2:3">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="367" spans="1:3">
       <c r="B367" t="s">
         <v>505</v>
       </c>
       <c r="C367" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="368" spans="1:3">
+      <c r="B368" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="368" spans="2:3">
-      <c r="B368" t="s">
-        <v>507</v>
-      </c>
       <c r="C368" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
     </row>
     <row r="369" spans="1:3">
       <c r="B369" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C369" t="s">
-        <v>230</v>
+        <v>30</v>
       </c>
     </row>
     <row r="370" spans="1:3">
       <c r="B370" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C370" t="s">
-        <v>511</v>
+        <v>30</v>
       </c>
     </row>
     <row r="371" spans="1:3">
       <c r="B371" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="C371" t="s">
-        <v>513</v>
+        <v>30</v>
       </c>
     </row>
     <row r="372" spans="1:3">
       <c r="B372" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="C372" t="s">
-        <v>319</v>
+        <v>511</v>
       </c>
     </row>
     <row r="373" spans="1:3">
       <c r="B373" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="C373" t="s">
-        <v>80</v>
+        <v>513</v>
       </c>
     </row>
     <row r="374" spans="1:3">
       <c r="B374" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C374" t="s">
-        <v>68</v>
+        <v>235</v>
       </c>
     </row>
     <row r="375" spans="1:3">
       <c r="B375" t="s">
+        <v>515</v>
+      </c>
+      <c r="C375" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="376" spans="1:3">
+      <c r="B376" t="s">
         <v>517</v>
       </c>
-      <c r="C375" t="s">
-        <v>70</v>
+      <c r="C376" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="377" spans="1:3">
-      <c r="A377" t="s">
-        <v>518</v>
-      </c>
       <c r="B377" t="s">
         <v>519</v>
       </c>
       <c r="C377" t="s">
-        <v>520</v>
+        <v>324</v>
       </c>
     </row>
     <row r="378" spans="1:3">
       <c r="B378" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C378" t="s">
-        <v>522</v>
+        <v>85</v>
       </c>
     </row>
     <row r="379" spans="1:3">
       <c r="B379" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C379" t="s">
-        <v>2</v>
+        <v>73</v>
       </c>
     </row>
     <row r="380" spans="1:3">
       <c r="B380" t="s">
+        <v>522</v>
+      </c>
+      <c r="C380" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="382" spans="1:3">
+      <c r="A382" t="s">
+        <v>523</v>
+      </c>
+      <c r="B382" t="s">
         <v>524</v>
       </c>
-      <c r="C380" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="381" spans="1:3">
-      <c r="B381" t="s">
+      <c r="C382" t="s">
         <v>525</v>
       </c>
-      <c r="C381" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="382" spans="1:3">
-      <c r="B382" t="s">
+    </row>
+    <row r="383" spans="1:3">
+      <c r="B383" t="s">
         <v>526</v>
       </c>
-      <c r="C382" t="s">
-        <v>25</v>
+      <c r="C383" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="384" spans="1:3">
-      <c r="A384" t="s">
-        <v>527</v>
-      </c>
       <c r="B384" t="s">
         <v>528</v>
       </c>
@@ -5060,10 +5080,15 @@
         <v>2</v>
       </c>
     </row>
+    <row r="385" spans="1:3">
+      <c r="B385" t="s">
+        <v>529</v>
+      </c>
+      <c r="C385" t="s">
+        <v>213</v>
+      </c>
+    </row>
     <row r="386" spans="1:3">
-      <c r="A386" t="s">
-        <v>529</v>
-      </c>
       <c r="B386" t="s">
         <v>530</v>
       </c>
@@ -5073,21 +5098,16 @@
     </row>
     <row r="387" spans="1:3">
       <c r="B387" t="s">
-        <v>207</v>
+        <v>531</v>
       </c>
       <c r="C387" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="388" spans="1:3">
-      <c r="B388" t="s">
-        <v>531</v>
-      </c>
-      <c r="C388" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="389" spans="1:3">
+      <c r="A389" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="389" spans="1:3">
       <c r="B389" t="s">
         <v>533</v>
       </c>
@@ -5095,92 +5115,87 @@
         <v>2</v>
       </c>
     </row>
-    <row r="390" spans="1:3">
-      <c r="B390" t="s">
+    <row r="391" spans="1:3">
+      <c r="A391" t="s">
         <v>534</v>
       </c>
-      <c r="C390" t="s">
+      <c r="B391" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="391" spans="1:3">
-      <c r="B391" t="s">
-        <v>536</v>
-      </c>
       <c r="C391" t="s">
-        <v>278</v>
+        <v>2</v>
       </c>
     </row>
     <row r="392" spans="1:3">
       <c r="B392" t="s">
-        <v>537</v>
+        <v>212</v>
       </c>
       <c r="C392" t="s">
-        <v>538</v>
+        <v>213</v>
       </c>
     </row>
     <row r="393" spans="1:3">
       <c r="B393" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C393" t="s">
-        <v>25</v>
+        <v>537</v>
       </c>
     </row>
     <row r="394" spans="1:3">
       <c r="B394" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C394" t="s">
-        <v>541</v>
+        <v>2</v>
       </c>
     </row>
     <row r="395" spans="1:3">
       <c r="B395" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C395" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="396" spans="1:3">
       <c r="B396" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="C396" t="s">
-        <v>2</v>
+        <v>283</v>
       </c>
     </row>
     <row r="397" spans="1:3">
       <c r="B397" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="C397" t="s">
-        <v>2</v>
+        <v>543</v>
       </c>
     </row>
     <row r="398" spans="1:3">
       <c r="B398" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C398" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="399" spans="1:3">
       <c r="B399" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C399" t="s">
-        <v>2</v>
+        <v>546</v>
       </c>
     </row>
     <row r="400" spans="1:3">
       <c r="B400" t="s">
+        <v>547</v>
+      </c>
+      <c r="C400" t="s">
         <v>548</v>
-      </c>
-      <c r="C400" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="401" spans="2:3">
@@ -5188,7 +5203,7 @@
         <v>549</v>
       </c>
       <c r="C401" t="s">
-        <v>532</v>
+        <v>2</v>
       </c>
     </row>
     <row r="402" spans="2:3">
@@ -5204,7 +5219,7 @@
         <v>551</v>
       </c>
       <c r="C403" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
     </row>
     <row r="404" spans="2:3">
@@ -5212,7 +5227,7 @@
         <v>552</v>
       </c>
       <c r="C404" t="s">
-        <v>535</v>
+        <v>2</v>
       </c>
     </row>
     <row r="405" spans="2:3">
@@ -5220,7 +5235,7 @@
         <v>553</v>
       </c>
       <c r="C405" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="406" spans="2:3">
@@ -5228,7 +5243,7 @@
         <v>554</v>
       </c>
       <c r="C406" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="407" spans="2:3">
@@ -5236,7 +5251,7 @@
         <v>555</v>
       </c>
       <c r="C407" t="s">
-        <v>208</v>
+        <v>2</v>
       </c>
     </row>
     <row r="408" spans="2:3">
@@ -5244,7 +5259,7 @@
         <v>556</v>
       </c>
       <c r="C408" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="409" spans="2:3">
@@ -5252,7 +5267,7 @@
         <v>557</v>
       </c>
       <c r="C409" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="410" spans="2:3">
@@ -5260,7 +5275,7 @@
         <v>558</v>
       </c>
       <c r="C410" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="411" spans="2:3">
@@ -5268,7 +5283,7 @@
         <v>559</v>
       </c>
       <c r="C411" t="s">
-        <v>2</v>
+        <v>543</v>
       </c>
     </row>
     <row r="412" spans="2:3">
@@ -5276,7 +5291,7 @@
         <v>560</v>
       </c>
       <c r="C412" t="s">
-        <v>27</v>
+        <v>213</v>
       </c>
     </row>
     <row r="413" spans="2:3">
@@ -5284,7 +5299,7 @@
         <v>561</v>
       </c>
       <c r="C413" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="414" spans="2:3">
@@ -5292,7 +5307,7 @@
         <v>562</v>
       </c>
       <c r="C414" t="s">
-        <v>2</v>
+        <v>548</v>
       </c>
     </row>
     <row r="415" spans="2:3">
@@ -5300,7 +5315,7 @@
         <v>563</v>
       </c>
       <c r="C415" t="s">
-        <v>532</v>
+        <v>2</v>
       </c>
     </row>
     <row r="416" spans="2:3">
@@ -5316,7 +5331,7 @@
         <v>565</v>
       </c>
       <c r="C417" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
     </row>
     <row r="418" spans="2:3">
@@ -5324,7 +5339,7 @@
         <v>566</v>
       </c>
       <c r="C418" t="s">
-        <v>535</v>
+        <v>2</v>
       </c>
     </row>
     <row r="419" spans="2:3">
@@ -5332,7 +5347,7 @@
         <v>567</v>
       </c>
       <c r="C419" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="420" spans="2:3">
@@ -5340,7 +5355,7 @@
         <v>568</v>
       </c>
       <c r="C420" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="421" spans="2:3">
@@ -5348,7 +5363,7 @@
         <v>569</v>
       </c>
       <c r="C421" t="s">
-        <v>416</v>
+        <v>2</v>
       </c>
     </row>
     <row r="422" spans="2:3">
@@ -5356,7 +5371,7 @@
         <v>570</v>
       </c>
       <c r="C422" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="423" spans="2:3">
@@ -5364,7 +5379,7 @@
         <v>571</v>
       </c>
       <c r="C423" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="424" spans="2:3">
@@ -5372,7 +5387,7 @@
         <v>572</v>
       </c>
       <c r="C424" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="425" spans="2:3">
@@ -5380,7 +5395,7 @@
         <v>573</v>
       </c>
       <c r="C425" t="s">
-        <v>2</v>
+        <v>543</v>
       </c>
     </row>
     <row r="426" spans="2:3">
@@ -5388,7 +5403,7 @@
         <v>574</v>
       </c>
       <c r="C426" t="s">
-        <v>27</v>
+        <v>421</v>
       </c>
     </row>
     <row r="427" spans="2:3">
@@ -5396,7 +5411,7 @@
         <v>575</v>
       </c>
       <c r="C427" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="428" spans="2:3">
@@ -5404,7 +5419,7 @@
         <v>576</v>
       </c>
       <c r="C428" t="s">
-        <v>2</v>
+        <v>548</v>
       </c>
     </row>
     <row r="429" spans="2:3">
@@ -5412,7 +5427,7 @@
         <v>577</v>
       </c>
       <c r="C429" t="s">
-        <v>532</v>
+        <v>2</v>
       </c>
     </row>
     <row r="430" spans="2:3">
@@ -5428,7 +5443,7 @@
         <v>579</v>
       </c>
       <c r="C431" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
     </row>
     <row r="432" spans="2:3">
@@ -5436,7 +5451,7 @@
         <v>580</v>
       </c>
       <c r="C432" t="s">
-        <v>535</v>
+        <v>2</v>
       </c>
     </row>
     <row r="433" spans="2:3">
@@ -5444,7 +5459,7 @@
         <v>581</v>
       </c>
       <c r="C433" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="434" spans="2:3">
@@ -5452,7 +5467,7 @@
         <v>582</v>
       </c>
       <c r="C434" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="435" spans="2:3">
@@ -5460,7 +5475,7 @@
         <v>583</v>
       </c>
       <c r="C435" t="s">
-        <v>319</v>
+        <v>2</v>
       </c>
     </row>
     <row r="436" spans="2:3">
@@ -5468,7 +5483,7 @@
         <v>584</v>
       </c>
       <c r="C436" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="437" spans="2:3">
@@ -5476,7 +5491,7 @@
         <v>585</v>
       </c>
       <c r="C437" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="438" spans="2:3">
@@ -5484,7 +5499,7 @@
         <v>586</v>
       </c>
       <c r="C438" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="439" spans="2:3">
@@ -5492,7 +5507,7 @@
         <v>587</v>
       </c>
       <c r="C439" t="s">
-        <v>2</v>
+        <v>543</v>
       </c>
     </row>
     <row r="440" spans="2:3">
@@ -5500,7 +5515,7 @@
         <v>588</v>
       </c>
       <c r="C440" t="s">
-        <v>27</v>
+        <v>324</v>
       </c>
     </row>
     <row r="441" spans="2:3">
@@ -5508,7 +5523,7 @@
         <v>589</v>
       </c>
       <c r="C441" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="442" spans="2:3">
@@ -5516,7 +5531,7 @@
         <v>590</v>
       </c>
       <c r="C442" t="s">
-        <v>2</v>
+        <v>548</v>
       </c>
     </row>
     <row r="443" spans="2:3">
@@ -5524,7 +5539,47 @@
         <v>591</v>
       </c>
       <c r="C443" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="444" spans="2:3">
+      <c r="B444" t="s">
         <v>592</v>
+      </c>
+      <c r="C444" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="445" spans="2:3">
+      <c r="B445" t="s">
+        <v>593</v>
+      </c>
+      <c r="C445" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="446" spans="2:3">
+      <c r="B446" t="s">
+        <v>594</v>
+      </c>
+      <c r="C446" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="447" spans="2:3">
+      <c r="B447" t="s">
+        <v>595</v>
+      </c>
+      <c r="C447" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="448" spans="2:3">
+      <c r="B448" t="s">
+        <v>596</v>
+      </c>
+      <c r="C448" t="s">
+        <v>597</v>
       </c>
     </row>
   </sheetData>

</xml_diff>